<commit_message>
added output_variables translation capability
</commit_message>
<xml_diff>
--- a/spec/files/discrete_variables.xlsx
+++ b/spec/files/discrete_variables.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19720" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12816" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
     <sheet name="Setup" sheetId="7" r:id="rId2"/>
     <sheet name="Variables" sheetId="2" r:id="rId3"/>
-    <sheet name="BCL Measure Data" sheetId="10" r:id="rId4"/>
+    <sheet name="Outputs" sheetId="11" r:id="rId4"/>
+    <sheet name="BCL Measure Data" sheetId="10" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$Y$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Y$13</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="489">
   <si>
     <t>type</t>
   </si>
@@ -1474,6 +1476,27 @@
   </si>
   <si>
     <t>['true','false']</t>
+  </si>
+  <si>
+    <t>Variable Display Name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>objective function</t>
+  </si>
+  <si>
+    <t>objective function target</t>
+  </si>
+  <si>
+    <t>true/false</t>
+  </si>
+  <si>
+    <t>(double)</t>
   </si>
 </sst>
 </file>
@@ -4161,7 +4184,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instructions"/>
@@ -4519,17 +4542,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.83203125" customWidth="1"/>
+    <col min="1" max="1" width="50.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -4553,17 +4576,17 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="21"/>
@@ -4572,7 +4595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1">
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>451</v>
       </c>
@@ -4581,7 +4604,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>452</v>
       </c>
@@ -4592,7 +4615,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>454</v>
       </c>
@@ -4611,7 +4634,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>457</v>
       </c>
@@ -4630,7 +4653,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="13" customFormat="1">
+    <row r="7" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>32</v>
       </c>
@@ -4639,7 +4662,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -4650,7 +4673,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -4658,7 +4681,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -4666,7 +4689,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="12" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>31</v>
       </c>
@@ -4677,7 +4700,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>462</v>
       </c>
@@ -4685,7 +4708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>463</v>
       </c>
@@ -4696,7 +4719,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -4704,7 +4727,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -4712,7 +4735,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>465</v>
       </c>
@@ -4721,7 +4744,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>38</v>
       </c>
@@ -4734,7 +4757,7 @@
       <c r="D20" s="12"/>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -4742,7 +4765,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>34</v>
       </c>
@@ -4759,7 +4782,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28">
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
@@ -4776,7 +4799,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>40</v>
       </c>
@@ -4820,34 +4843,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="5"/>
-    <col min="10" max="13" width="11.5" style="1"/>
+    <col min="9" max="9" width="11.44140625" style="5"/>
+    <col min="10" max="13" width="11.44140625" style="1"/>
     <col min="14" max="14" width="13.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" style="1"/>
-    <col min="18" max="18" width="46.1640625" style="1" customWidth="1"/>
-    <col min="19" max="21" width="11.5" style="1"/>
+    <col min="16" max="16" width="16.77734375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" style="1"/>
+    <col min="18" max="18" width="46.109375" style="1" customWidth="1"/>
+    <col min="19" max="21" width="11.44140625" style="1"/>
     <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.5" style="1"/>
+    <col min="23" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18">
+    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -4881,7 +4904,7 @@
       <c r="W1" s="29"/>
       <c r="X1" s="29"/>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="15">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -4894,7 +4917,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:24" s="16" customFormat="1" ht="45">
+    <row r="3" spans="1:24" s="16" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -4965,7 +4988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -4991,7 +5014,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>24</v>
@@ -5024,7 +5047,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6" t="s">
         <v>25</v>
@@ -5063,7 +5086,7 @@
       </c>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7" t="s">
         <v>24</v>
@@ -5093,7 +5116,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8" t="s">
         <v>24</v>
@@ -5123,7 +5146,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9" t="s">
         <v>24</v>
@@ -5153,7 +5176,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10" t="s">
         <v>24</v>
@@ -5185,7 +5208,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11" t="s">
         <v>24</v>
@@ -5215,7 +5238,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12" t="s">
         <v>24</v>
@@ -5245,7 +5268,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13" t="s">
         <v>24</v>
@@ -5275,7 +5298,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:24" customFormat="1">
+    <row r="14" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -5289,7 +5312,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:24" customFormat="1">
+    <row r="15" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -5312,7 +5335,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:24" customFormat="1">
+    <row r="16" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -5350,7 +5373,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:16" customFormat="1">
+    <row r="17" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>24</v>
       </c>
@@ -5370,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" customFormat="1">
+    <row r="18" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -5390,7 +5413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" customFormat="1">
+    <row r="19" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -5410,7 +5433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" customFormat="1" ht="15">
+    <row r="20" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="b">
         <v>1</v>
       </c>
@@ -5436,7 +5459,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" customFormat="1" ht="15">
+    <row r="21" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
       <c r="B21" s="20" t="s">
         <v>25</v>
@@ -5477,7 +5500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:16" customFormat="1" ht="15">
+    <row r="22" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>25</v>
@@ -5518,7 +5541,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:16" customFormat="1" ht="15">
+    <row r="23" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>25</v>
@@ -5550,7 +5573,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="24" spans="1:16" customFormat="1" ht="15">
+    <row r="24" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="b">
         <v>1</v>
       </c>
@@ -5569,7 +5592,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:16" customFormat="1" ht="15">
+    <row r="25" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>25</v>
@@ -5610,7 +5633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" customFormat="1" ht="15">
+    <row r="26" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>24</v>
@@ -5633,7 +5656,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:16" customFormat="1" ht="15">
+    <row r="27" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>24</v>
@@ -5656,7 +5679,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:16" customFormat="1" ht="15">
+    <row r="28" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>24</v>
@@ -5679,7 +5702,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:16" customFormat="1" ht="15">
+    <row r="29" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="b">
         <v>1</v>
       </c>
@@ -5698,7 +5721,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:16" customFormat="1" ht="15">
+    <row r="30" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>25</v>
@@ -5739,7 +5762,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:16" customFormat="1" ht="15">
+    <row r="31" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="20"/>
       <c r="B31" s="20" t="s">
         <v>24</v>
@@ -5762,7 +5785,7 @@
       </c>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:16" customFormat="1" ht="15">
+    <row r="32" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>24</v>
@@ -5785,7 +5808,7 @@
       </c>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:16" customFormat="1" ht="15">
+    <row r="33" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>24</v>
@@ -5808,7 +5831,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:16" customFormat="1" ht="15">
+    <row r="34" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="b">
         <v>1</v>
       </c>
@@ -5827,7 +5850,7 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:16" customFormat="1" ht="15">
+    <row r="35" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>24</v>
@@ -5852,7 +5875,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:16" customFormat="1" ht="15">
+    <row r="36" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>25</v>
@@ -5898,25 +5921,549 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="5"/>
+    <col min="10" max="13" width="11.44140625" style="1"/>
+    <col min="14" max="14" width="13.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.77734375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" style="1"/>
+    <col min="18" max="18" width="46.109375" style="1" customWidth="1"/>
+    <col min="19" max="21" width="11.44140625" style="1"/>
+    <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+    </row>
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:24" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7" s="15"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:24" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:24" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="19"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+    </row>
+    <row r="32" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+    </row>
+    <row r="33" spans="1:15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="1:15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+    </row>
+    <row r="35" spans="1:15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+    </row>
+    <row r="36" spans="1:15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:Y13"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I327"/>
   <sheetViews>
     <sheetView topLeftCell="C49" workbookViewId="0">
       <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="b">
         <v>0</v>
       </c>
@@ -5935,7 +6482,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
         <v>24</v>
@@ -5956,7 +6503,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
         <v>24</v>
@@ -5979,7 +6526,7 @@
       </c>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="20" t="s">
         <v>24</v>
@@ -6002,7 +6549,7 @@
       </c>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="20" t="s">
         <v>24</v>
@@ -6025,7 +6572,7 @@
       </c>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="20" t="s">
         <v>24</v>
@@ -6048,7 +6595,7 @@
       </c>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="20" t="s">
         <v>24</v>
@@ -6071,7 +6618,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="20" t="s">
         <v>24</v>
@@ -6094,7 +6641,7 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="20" t="s">
         <v>24</v>
@@ -6117,7 +6664,7 @@
       </c>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
         <v>24</v>
@@ -6140,7 +6687,7 @@
       </c>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="b">
         <v>0</v>
       </c>
@@ -6159,7 +6706,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="20" t="s">
         <v>24</v>
@@ -6180,7 +6727,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="20" t="s">
         <v>24</v>
@@ -6203,7 +6750,7 @@
       </c>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="20" t="s">
         <v>24</v>
@@ -6226,7 +6773,7 @@
       </c>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="20" t="s">
         <v>24</v>
@@ -6249,7 +6796,7 @@
       </c>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" ht="15">
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="20" t="s">
         <v>24</v>
@@ -6272,7 +6819,7 @@
       </c>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9" ht="15">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="20" t="s">
         <v>24</v>
@@ -6295,7 +6842,7 @@
       </c>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="15">
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="20" t="s">
         <v>24</v>
@@ -6318,7 +6865,7 @@
       </c>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="20" t="s">
         <v>24</v>
@@ -6341,7 +6888,7 @@
       </c>
       <c r="I19" s="20"/>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
         <v>24</v>
@@ -6364,7 +6911,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:9" ht="15">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="b">
         <v>0</v>
       </c>
@@ -6383,7 +6930,7 @@
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:9" ht="15">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>24</v>
@@ -6406,7 +6953,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>24</v>
@@ -6429,7 +6976,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:9" ht="15">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="20" t="s">
         <v>24</v>
@@ -6452,7 +6999,7 @@
       </c>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:9" ht="15">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>24</v>
@@ -6475,7 +7022,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:9" ht="15">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>24</v>
@@ -6498,7 +7045,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="15">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>24</v>
@@ -6521,7 +7068,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="15">
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>24</v>
@@ -6544,7 +7091,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="15">
+    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
       <c r="B29" s="20" t="s">
         <v>24</v>
@@ -6567,7 +7114,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" ht="15">
+    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>24</v>
@@ -6590,7 +7137,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="15">
+    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="b">
         <v>0</v>
       </c>
@@ -6609,7 +7156,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="15">
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>24</v>
@@ -6630,7 +7177,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" ht="15">
+    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>24</v>
@@ -6653,7 +7200,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" ht="15">
+    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="20" t="s">
         <v>24</v>
@@ -6676,7 +7223,7 @@
       </c>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="15">
+    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>24</v>
@@ -6699,7 +7246,7 @@
       </c>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" ht="15">
+    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>24</v>
@@ -6722,7 +7269,7 @@
       </c>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" ht="15">
+    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="20"/>
       <c r="B37" s="20" t="s">
         <v>24</v>
@@ -6745,7 +7292,7 @@
       </c>
       <c r="I37" s="20"/>
     </row>
-    <row r="38" spans="1:9" ht="15">
+    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="20" t="s">
         <v>24</v>
@@ -6768,7 +7315,7 @@
       </c>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" ht="15">
+    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="20" t="s">
         <v>24</v>
@@ -6791,7 +7338,7 @@
       </c>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" ht="15">
+    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="20" t="s">
         <v>24</v>
@@ -6814,7 +7361,7 @@
       </c>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" ht="15">
+    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="b">
         <v>0</v>
       </c>
@@ -6833,7 +7380,7 @@
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
     </row>
-    <row r="42" spans="1:9" ht="15">
+    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
       <c r="B42" s="20" t="s">
         <v>24</v>
@@ -6854,7 +7401,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" ht="15">
+    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="20" t="s">
         <v>24</v>
@@ -6877,7 +7424,7 @@
       </c>
       <c r="I43" s="20"/>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="20" t="s">
         <v>24</v>
@@ -6900,7 +7447,7 @@
       </c>
       <c r="I44" s="20"/>
     </row>
-    <row r="45" spans="1:9" ht="15">
+    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="20"/>
       <c r="B45" s="20" t="s">
         <v>24</v>
@@ -6923,7 +7470,7 @@
       </c>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" ht="15">
+    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="20"/>
       <c r="B46" s="20" t="s">
         <v>24</v>
@@ -6946,7 +7493,7 @@
       </c>
       <c r="I46" s="20"/>
     </row>
-    <row r="47" spans="1:9" ht="15">
+    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20"/>
       <c r="B47" s="20" t="s">
         <v>24</v>
@@ -6969,7 +7516,7 @@
       </c>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" ht="15">
+    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="20"/>
       <c r="B48" s="20" t="s">
         <v>24</v>
@@ -6992,7 +7539,7 @@
       </c>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="1:9" ht="15">
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="20"/>
       <c r="B49" s="20" t="s">
         <v>24</v>
@@ -7015,7 +7562,7 @@
       </c>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="1:9" ht="15">
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="20"/>
       <c r="B50" s="20" t="s">
         <v>24</v>
@@ -7038,7 +7585,7 @@
       </c>
       <c r="I50" s="20"/>
     </row>
-    <row r="51" spans="1:9" ht="15">
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="b">
         <v>0</v>
       </c>
@@ -7057,7 +7604,7 @@
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="1:9" ht="15">
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="20"/>
       <c r="B52" s="20" t="s">
         <v>24</v>
@@ -7078,7 +7625,7 @@
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="15">
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="20"/>
       <c r="B53" s="20" t="s">
         <v>24</v>
@@ -7101,7 +7648,7 @@
       </c>
       <c r="I53" s="20"/>
     </row>
-    <row r="54" spans="1:9" ht="15">
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="20" t="s">
         <v>24</v>
@@ -7124,7 +7671,7 @@
       </c>
       <c r="I54" s="20"/>
     </row>
-    <row r="55" spans="1:9" ht="15">
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="20"/>
       <c r="B55" s="20" t="s">
         <v>24</v>
@@ -7147,7 +7694,7 @@
       </c>
       <c r="I55" s="20"/>
     </row>
-    <row r="56" spans="1:9" ht="15">
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="20"/>
       <c r="B56" s="20" t="s">
         <v>24</v>
@@ -7170,7 +7717,7 @@
       </c>
       <c r="I56" s="20"/>
     </row>
-    <row r="57" spans="1:9" ht="15">
+    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="B57" s="20" t="s">
         <v>24</v>
@@ -7193,7 +7740,7 @@
       </c>
       <c r="I57" s="20"/>
     </row>
-    <row r="58" spans="1:9" ht="15">
+    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="20"/>
       <c r="B58" s="20" t="s">
         <v>24</v>
@@ -7216,7 +7763,7 @@
       </c>
       <c r="I58" s="20"/>
     </row>
-    <row r="59" spans="1:9" ht="15">
+    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="20"/>
       <c r="B59" s="20" t="s">
         <v>24</v>
@@ -7239,7 +7786,7 @@
       </c>
       <c r="I59" s="20"/>
     </row>
-    <row r="60" spans="1:9" ht="15">
+    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="20"/>
       <c r="B60" s="20" t="s">
         <v>24</v>
@@ -7262,7 +7809,7 @@
       </c>
       <c r="I60" s="20"/>
     </row>
-    <row r="61" spans="1:9" ht="15">
+    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="b">
         <v>0</v>
       </c>
@@ -7281,7 +7828,7 @@
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
     </row>
-    <row r="62" spans="1:9" ht="15">
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="20"/>
       <c r="B62" s="20" t="s">
         <v>24</v>
@@ -7302,7 +7849,7 @@
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
     </row>
-    <row r="63" spans="1:9" ht="15">
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="20"/>
       <c r="B63" s="20" t="s">
         <v>24</v>
@@ -7327,7 +7874,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15">
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
       <c r="B64" s="20" t="s">
         <v>24</v>
@@ -7350,7 +7897,7 @@
       </c>
       <c r="I64" s="20"/>
     </row>
-    <row r="65" spans="1:9" ht="15">
+    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="20"/>
       <c r="B65" s="20" t="s">
         <v>24</v>
@@ -7373,7 +7920,7 @@
       </c>
       <c r="I65" s="20"/>
     </row>
-    <row r="66" spans="1:9" ht="15">
+    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="20"/>
       <c r="B66" s="20" t="s">
         <v>24</v>
@@ -7396,7 +7943,7 @@
       </c>
       <c r="I66" s="20"/>
     </row>
-    <row r="67" spans="1:9" ht="15">
+    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="20"/>
       <c r="B67" s="20" t="s">
         <v>24</v>
@@ -7419,7 +7966,7 @@
       </c>
       <c r="I67" s="20"/>
     </row>
-    <row r="68" spans="1:9" ht="15">
+    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="20"/>
       <c r="B68" s="20" t="s">
         <v>24</v>
@@ -7442,7 +7989,7 @@
       </c>
       <c r="I68" s="20"/>
     </row>
-    <row r="69" spans="1:9" ht="15">
+    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="20"/>
       <c r="B69" s="20" t="s">
         <v>24</v>
@@ -7465,7 +8012,7 @@
       </c>
       <c r="I69" s="20"/>
     </row>
-    <row r="70" spans="1:9" ht="15">
+    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="20"/>
       <c r="B70" s="20" t="s">
         <v>24</v>
@@ -7488,7 +8035,7 @@
       </c>
       <c r="I70" s="20"/>
     </row>
-    <row r="71" spans="1:9" ht="15">
+    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="20"/>
       <c r="B71" s="20" t="s">
         <v>24</v>
@@ -7511,7 +8058,7 @@
       </c>
       <c r="I71" s="20"/>
     </row>
-    <row r="72" spans="1:9" ht="15">
+    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="b">
         <v>0</v>
       </c>
@@ -7530,7 +8077,7 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
     </row>
-    <row r="73" spans="1:9" ht="15">
+    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="20"/>
       <c r="B73" s="20" t="s">
         <v>24</v>
@@ -7551,7 +8098,7 @@
       <c r="H73" s="20"/>
       <c r="I73" s="20"/>
     </row>
-    <row r="74" spans="1:9" ht="15">
+    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="20"/>
       <c r="B74" s="20" t="s">
         <v>24</v>
@@ -7574,7 +8121,7 @@
       </c>
       <c r="I74" s="20"/>
     </row>
-    <row r="75" spans="1:9" ht="15">
+    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="20"/>
       <c r="B75" s="20" t="s">
         <v>24</v>
@@ -7599,7 +8146,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15">
+    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="20"/>
       <c r="B76" s="20" t="s">
         <v>24</v>
@@ -7622,7 +8169,7 @@
       </c>
       <c r="I76" s="20"/>
     </row>
-    <row r="77" spans="1:9" ht="15">
+    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="20"/>
       <c r="B77" s="20" t="s">
         <v>24</v>
@@ -7645,7 +8192,7 @@
       </c>
       <c r="I77" s="20"/>
     </row>
-    <row r="78" spans="1:9" ht="15">
+    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="20"/>
       <c r="B78" s="20" t="s">
         <v>24</v>
@@ -7668,7 +8215,7 @@
       </c>
       <c r="I78" s="20"/>
     </row>
-    <row r="79" spans="1:9" ht="15">
+    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="20"/>
       <c r="B79" s="20" t="s">
         <v>24</v>
@@ -7691,7 +8238,7 @@
       </c>
       <c r="I79" s="20"/>
     </row>
-    <row r="80" spans="1:9" ht="15">
+    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="20"/>
       <c r="B80" s="20" t="s">
         <v>24</v>
@@ -7714,7 +8261,7 @@
       </c>
       <c r="I80" s="20"/>
     </row>
-    <row r="81" spans="1:9" ht="15">
+    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="20"/>
       <c r="B81" s="20" t="s">
         <v>24</v>
@@ -7737,7 +8284,7 @@
       </c>
       <c r="I81" s="20"/>
     </row>
-    <row r="82" spans="1:9" ht="15">
+    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="20"/>
       <c r="B82" s="20" t="s">
         <v>24</v>
@@ -7760,7 +8307,7 @@
       </c>
       <c r="I82" s="20"/>
     </row>
-    <row r="83" spans="1:9" ht="15">
+    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="20"/>
       <c r="B83" s="20" t="s">
         <v>24</v>
@@ -7783,7 +8330,7 @@
       </c>
       <c r="I83" s="20"/>
     </row>
-    <row r="84" spans="1:9" ht="15">
+    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="20"/>
       <c r="B84" s="20" t="s">
         <v>24</v>
@@ -7806,7 +8353,7 @@
       </c>
       <c r="I84" s="20"/>
     </row>
-    <row r="85" spans="1:9" ht="15">
+    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="20"/>
       <c r="B85" s="20" t="s">
         <v>24</v>
@@ -7829,7 +8376,7 @@
       </c>
       <c r="I85" s="20"/>
     </row>
-    <row r="86" spans="1:9" ht="15">
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="20" t="b">
         <v>0</v>
       </c>
@@ -7848,7 +8395,7 @@
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
     </row>
-    <row r="87" spans="1:9" ht="15">
+    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="20"/>
       <c r="B87" s="20" t="s">
         <v>24</v>
@@ -7871,7 +8418,7 @@
       </c>
       <c r="I87" s="20"/>
     </row>
-    <row r="88" spans="1:9" ht="15">
+    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="20"/>
       <c r="B88" s="20" t="s">
         <v>24</v>
@@ -7894,7 +8441,7 @@
       </c>
       <c r="I88" s="20"/>
     </row>
-    <row r="89" spans="1:9" ht="15">
+    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="20"/>
       <c r="B89" s="20" t="s">
         <v>24</v>
@@ -7917,7 +8464,7 @@
       </c>
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="1:9" ht="15">
+    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="20"/>
       <c r="B90" s="20" t="s">
         <v>24</v>
@@ -7940,7 +8487,7 @@
       </c>
       <c r="I90" s="20"/>
     </row>
-    <row r="91" spans="1:9" ht="15">
+    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="20"/>
       <c r="B91" s="20" t="s">
         <v>24</v>
@@ -7963,7 +8510,7 @@
       </c>
       <c r="I91" s="20"/>
     </row>
-    <row r="92" spans="1:9" ht="15">
+    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="20"/>
       <c r="B92" s="20" t="s">
         <v>24</v>
@@ -7986,7 +8533,7 @@
       </c>
       <c r="I92" s="20"/>
     </row>
-    <row r="93" spans="1:9" ht="15">
+    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="20"/>
       <c r="B93" s="20" t="s">
         <v>24</v>
@@ -8009,7 +8556,7 @@
       </c>
       <c r="I93" s="20"/>
     </row>
-    <row r="94" spans="1:9" ht="15">
+    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="20"/>
       <c r="B94" s="20" t="s">
         <v>24</v>
@@ -8032,7 +8579,7 @@
       </c>
       <c r="I94" s="20"/>
     </row>
-    <row r="95" spans="1:9" ht="15">
+    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="20"/>
       <c r="B95" s="20" t="s">
         <v>24</v>
@@ -8055,7 +8602,7 @@
       </c>
       <c r="I95" s="20"/>
     </row>
-    <row r="96" spans="1:9" ht="15">
+    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="20"/>
       <c r="B96" s="20" t="s">
         <v>24</v>
@@ -8078,7 +8625,7 @@
       </c>
       <c r="I96" s="20"/>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="20" t="b">
         <v>0</v>
       </c>
@@ -8097,7 +8644,7 @@
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
     </row>
-    <row r="98" spans="1:9" ht="15">
+    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="20"/>
       <c r="B98" s="20" t="s">
         <v>24</v>
@@ -8122,7 +8669,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15">
+    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="20" t="b">
         <v>0</v>
       </c>
@@ -8141,7 +8688,7 @@
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
     </row>
-    <row r="100" spans="1:9" ht="15">
+    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="20"/>
       <c r="B100" s="20" t="s">
         <v>24</v>
@@ -8162,7 +8709,7 @@
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
     </row>
-    <row r="101" spans="1:9" ht="19" customHeight="1">
+    <row r="101" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="20"/>
       <c r="B101" s="20" t="s">
         <v>24</v>
@@ -8187,7 +8734,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15">
+    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="20" t="b">
         <v>0</v>
       </c>
@@ -8206,7 +8753,7 @@
       <c r="H102" s="20"/>
       <c r="I102" s="20"/>
     </row>
-    <row r="103" spans="1:9" ht="15">
+    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="20"/>
       <c r="B103" s="20" t="s">
         <v>24</v>
@@ -8229,7 +8776,7 @@
       </c>
       <c r="I103" s="20"/>
     </row>
-    <row r="104" spans="1:9" ht="15">
+    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="20"/>
       <c r="B104" s="20" t="s">
         <v>24</v>
@@ -8254,7 +8801,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15">
+    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="20"/>
       <c r="B105" s="20" t="s">
         <v>24</v>
@@ -8277,7 +8824,7 @@
       </c>
       <c r="I105" s="20"/>
     </row>
-    <row r="106" spans="1:9" ht="15">
+    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="20"/>
       <c r="B106" s="20" t="s">
         <v>24</v>
@@ -8298,7 +8845,7 @@
       <c r="H106" s="20"/>
       <c r="I106" s="20"/>
     </row>
-    <row r="107" spans="1:9" ht="15">
+    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="20" t="b">
         <v>0</v>
       </c>
@@ -8317,7 +8864,7 @@
       <c r="H107" s="20"/>
       <c r="I107" s="20"/>
     </row>
-    <row r="108" spans="1:9" ht="15">
+    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="20"/>
       <c r="B108" s="20" t="s">
         <v>24</v>
@@ -8342,7 +8889,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15">
+    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="20"/>
       <c r="B109" s="20" t="s">
         <v>24</v>
@@ -8365,7 +8912,7 @@
       </c>
       <c r="I109" s="20"/>
     </row>
-    <row r="110" spans="1:9" ht="15">
+    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="20"/>
       <c r="B110" s="20" t="s">
         <v>24</v>
@@ -8388,7 +8935,7 @@
       </c>
       <c r="I110" s="20"/>
     </row>
-    <row r="111" spans="1:9" ht="15">
+    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="20"/>
       <c r="B111" s="20" t="s">
         <v>24</v>
@@ -8411,7 +8958,7 @@
       </c>
       <c r="I111" s="20"/>
     </row>
-    <row r="112" spans="1:9" ht="15">
+    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="20"/>
       <c r="B112" s="20" t="s">
         <v>24</v>
@@ -8434,7 +8981,7 @@
       </c>
       <c r="I112" s="20"/>
     </row>
-    <row r="113" spans="1:9" ht="15">
+    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="20"/>
       <c r="B113" s="20" t="s">
         <v>24</v>
@@ -8457,7 +9004,7 @@
       </c>
       <c r="I113" s="20"/>
     </row>
-    <row r="114" spans="1:9" ht="15">
+    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="20"/>
       <c r="B114" s="20" t="s">
         <v>24</v>
@@ -8480,7 +9027,7 @@
       </c>
       <c r="I114" s="20"/>
     </row>
-    <row r="115" spans="1:9" ht="15">
+    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="b">
         <v>0</v>
       </c>
@@ -8499,7 +9046,7 @@
       <c r="H115" s="20"/>
       <c r="I115" s="20"/>
     </row>
-    <row r="116" spans="1:9" ht="15">
+    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="20"/>
       <c r="B116" s="20" t="s">
         <v>24</v>
@@ -8522,7 +9069,7 @@
       </c>
       <c r="I116" s="20"/>
     </row>
-    <row r="117" spans="1:9" ht="15">
+    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="20"/>
       <c r="B117" s="20" t="s">
         <v>24</v>
@@ -8545,7 +9092,7 @@
       </c>
       <c r="I117" s="20"/>
     </row>
-    <row r="118" spans="1:9" ht="15">
+    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="20"/>
       <c r="B118" s="20" t="s">
         <v>24</v>
@@ -8568,7 +9115,7 @@
       </c>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" ht="15">
+    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="20" t="b">
         <v>0</v>
       </c>
@@ -8587,7 +9134,7 @@
       <c r="H119" s="20"/>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="15">
+    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="20"/>
       <c r="B120" s="20" t="s">
         <v>24</v>
@@ -8610,7 +9157,7 @@
       </c>
       <c r="I120" s="20"/>
     </row>
-    <row r="121" spans="1:9" ht="15">
+    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="20"/>
       <c r="B121" s="20" t="s">
         <v>24</v>
@@ -8633,7 +9180,7 @@
       </c>
       <c r="I121" s="20"/>
     </row>
-    <row r="122" spans="1:9" ht="15">
+    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="20"/>
       <c r="B122" s="20" t="s">
         <v>24</v>
@@ -8656,7 +9203,7 @@
       </c>
       <c r="I122" s="20"/>
     </row>
-    <row r="123" spans="1:9" ht="15">
+    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="20"/>
       <c r="B123" s="20" t="s">
         <v>24</v>
@@ -8679,7 +9226,7 @@
       </c>
       <c r="I123" s="20"/>
     </row>
-    <row r="124" spans="1:9" ht="15">
+    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="20"/>
       <c r="B124" s="20" t="s">
         <v>24</v>
@@ -8702,7 +9249,7 @@
       </c>
       <c r="I124" s="20"/>
     </row>
-    <row r="125" spans="1:9" ht="15">
+    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="20"/>
       <c r="B125" s="20" t="s">
         <v>24</v>
@@ -8725,7 +9272,7 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:9" ht="15">
+    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="20" t="b">
         <v>0</v>
       </c>
@@ -8744,7 +9291,7 @@
       <c r="H126" s="20"/>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="1:9" ht="15">
+    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="20"/>
       <c r="B127" s="20" t="s">
         <v>24</v>
@@ -8769,7 +9316,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15">
+    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="20"/>
       <c r="B128" s="20" t="s">
         <v>24</v>
@@ -8792,7 +9339,7 @@
       </c>
       <c r="I128" s="20"/>
     </row>
-    <row r="129" spans="1:9" ht="15">
+    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="20"/>
       <c r="B129" s="20" t="s">
         <v>24</v>
@@ -8815,7 +9362,7 @@
       </c>
       <c r="I129" s="20"/>
     </row>
-    <row r="130" spans="1:9" ht="15">
+    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="20"/>
       <c r="B130" s="20" t="s">
         <v>24</v>
@@ -8838,7 +9385,7 @@
       </c>
       <c r="I130" s="20"/>
     </row>
-    <row r="131" spans="1:9" ht="15">
+    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="20"/>
       <c r="B131" s="20" t="s">
         <v>24</v>
@@ -8861,7 +9408,7 @@
       </c>
       <c r="I131" s="20"/>
     </row>
-    <row r="132" spans="1:9" ht="15">
+    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="20"/>
       <c r="B132" s="20" t="s">
         <v>24</v>
@@ -8884,7 +9431,7 @@
       </c>
       <c r="I132" s="20"/>
     </row>
-    <row r="133" spans="1:9" ht="15">
+    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="20"/>
       <c r="B133" s="20" t="s">
         <v>24</v>
@@ -8907,7 +9454,7 @@
       </c>
       <c r="I133" s="20"/>
     </row>
-    <row r="134" spans="1:9" ht="15">
+    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="20"/>
       <c r="B134" s="20" t="s">
         <v>24</v>
@@ -8930,7 +9477,7 @@
       </c>
       <c r="I134" s="20"/>
     </row>
-    <row r="135" spans="1:9" ht="15">
+    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="20"/>
       <c r="B135" s="20" t="s">
         <v>24</v>
@@ -8953,7 +9500,7 @@
       </c>
       <c r="I135" s="20"/>
     </row>
-    <row r="136" spans="1:9" ht="15">
+    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="20" t="b">
         <v>0</v>
       </c>
@@ -8972,7 +9519,7 @@
       <c r="H136" s="20"/>
       <c r="I136" s="20"/>
     </row>
-    <row r="137" spans="1:9" ht="15">
+    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="20"/>
       <c r="B137" s="20" t="s">
         <v>24</v>
@@ -8997,7 +9544,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15">
+    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="20"/>
       <c r="B138" s="20" t="s">
         <v>24</v>
@@ -9018,7 +9565,7 @@
       <c r="H138" s="20"/>
       <c r="I138" s="20"/>
     </row>
-    <row r="139" spans="1:9" ht="15">
+    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="20"/>
       <c r="B139" s="20" t="s">
         <v>24</v>
@@ -9041,7 +9588,7 @@
       </c>
       <c r="I139" s="20"/>
     </row>
-    <row r="140" spans="1:9" ht="15">
+    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="20"/>
       <c r="B140" s="20" t="s">
         <v>24</v>
@@ -9064,7 +9611,7 @@
       </c>
       <c r="I140" s="20"/>
     </row>
-    <row r="141" spans="1:9" ht="15">
+    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="20"/>
       <c r="B141" s="20" t="s">
         <v>24</v>
@@ -9087,7 +9634,7 @@
       </c>
       <c r="I141" s="20"/>
     </row>
-    <row r="142" spans="1:9" ht="15">
+    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="20"/>
       <c r="B142" s="20" t="s">
         <v>24</v>
@@ -9110,7 +9657,7 @@
       </c>
       <c r="I142" s="20"/>
     </row>
-    <row r="143" spans="1:9" ht="15">
+    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="20"/>
       <c r="B143" s="20" t="s">
         <v>24</v>
@@ -9133,7 +9680,7 @@
       </c>
       <c r="I143" s="20"/>
     </row>
-    <row r="144" spans="1:9" ht="15">
+    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="20"/>
       <c r="B144" s="20" t="s">
         <v>24</v>
@@ -9156,7 +9703,7 @@
       </c>
       <c r="I144" s="20"/>
     </row>
-    <row r="145" spans="1:9" ht="15">
+    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="20"/>
       <c r="B145" s="20" t="s">
         <v>24</v>
@@ -9179,7 +9726,7 @@
       </c>
       <c r="I145" s="20"/>
     </row>
-    <row r="146" spans="1:9" ht="15">
+    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="20"/>
       <c r="B146" s="20" t="s">
         <v>24</v>
@@ -9202,7 +9749,7 @@
       </c>
       <c r="I146" s="20"/>
     </row>
-    <row r="147" spans="1:9" ht="15">
+    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="20"/>
       <c r="B147" s="20" t="s">
         <v>24</v>
@@ -9225,7 +9772,7 @@
       </c>
       <c r="I147" s="20"/>
     </row>
-    <row r="148" spans="1:9" ht="15">
+    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="20"/>
       <c r="B148" s="20" t="s">
         <v>24</v>
@@ -9248,7 +9795,7 @@
       </c>
       <c r="I148" s="20"/>
     </row>
-    <row r="149" spans="1:9" ht="15">
+    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="20"/>
       <c r="B149" s="20" t="s">
         <v>24</v>
@@ -9271,7 +9818,7 @@
       </c>
       <c r="I149" s="20"/>
     </row>
-    <row r="150" spans="1:9" ht="15">
+    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="20"/>
       <c r="B150" s="20" t="s">
         <v>24</v>
@@ -9294,7 +9841,7 @@
       </c>
       <c r="I150" s="20"/>
     </row>
-    <row r="151" spans="1:9" ht="15">
+    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="20" t="b">
         <v>0</v>
       </c>
@@ -9313,7 +9860,7 @@
       <c r="H151" s="20"/>
       <c r="I151" s="20"/>
     </row>
-    <row r="152" spans="1:9" ht="15">
+    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="20"/>
       <c r="B152" s="20" t="s">
         <v>24</v>
@@ -9336,7 +9883,7 @@
       </c>
       <c r="I152" s="20"/>
     </row>
-    <row r="153" spans="1:9" ht="15">
+    <row r="153" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="20" t="b">
         <v>0</v>
       </c>
@@ -9355,7 +9902,7 @@
       <c r="H153" s="20"/>
       <c r="I153" s="20"/>
     </row>
-    <row r="154" spans="1:9" ht="15">
+    <row r="154" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="20"/>
       <c r="B154" s="20" t="s">
         <v>24</v>
@@ -9378,7 +9925,7 @@
       </c>
       <c r="I154" s="20"/>
     </row>
-    <row r="155" spans="1:9" ht="15">
+    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="20"/>
       <c r="B155" s="20" t="s">
         <v>24</v>
@@ -9401,7 +9948,7 @@
       </c>
       <c r="I155" s="20"/>
     </row>
-    <row r="156" spans="1:9" ht="15">
+    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="20" t="b">
         <v>0</v>
       </c>
@@ -9420,7 +9967,7 @@
       <c r="H156" s="20"/>
       <c r="I156" s="20"/>
     </row>
-    <row r="157" spans="1:9" ht="15">
+    <row r="157" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="20"/>
       <c r="B157" s="20" t="s">
         <v>24</v>
@@ -9445,7 +9992,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15">
+    <row r="158" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="20"/>
       <c r="B158" s="20" t="s">
         <v>24</v>
@@ -9468,7 +10015,7 @@
       </c>
       <c r="I158" s="20"/>
     </row>
-    <row r="159" spans="1:9" ht="15">
+    <row r="159" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="20"/>
       <c r="B159" s="20" t="s">
         <v>24</v>
@@ -9491,7 +10038,7 @@
       </c>
       <c r="I159" s="20"/>
     </row>
-    <row r="160" spans="1:9" ht="15">
+    <row r="160" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="20"/>
       <c r="B160" s="20" t="s">
         <v>24</v>
@@ -9514,7 +10061,7 @@
       </c>
       <c r="I160" s="20"/>
     </row>
-    <row r="161" spans="1:9" ht="15">
+    <row r="161" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="20"/>
       <c r="B161" s="20" t="s">
         <v>24</v>
@@ -9537,7 +10084,7 @@
       </c>
       <c r="I161" s="20"/>
     </row>
-    <row r="162" spans="1:9" ht="15">
+    <row r="162" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="20"/>
       <c r="B162" s="20" t="s">
         <v>24</v>
@@ -9560,7 +10107,7 @@
       </c>
       <c r="I162" s="20"/>
     </row>
-    <row r="163" spans="1:9" ht="15">
+    <row r="163" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="20"/>
       <c r="B163" s="20" t="s">
         <v>24</v>
@@ -9583,7 +10130,7 @@
       </c>
       <c r="I163" s="20"/>
     </row>
-    <row r="164" spans="1:9" ht="15">
+    <row r="164" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="20"/>
       <c r="B164" s="20" t="s">
         <v>24</v>
@@ -9606,7 +10153,7 @@
       </c>
       <c r="I164" s="20"/>
     </row>
-    <row r="165" spans="1:9" ht="15">
+    <row r="165" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="20"/>
       <c r="B165" s="20" t="s">
         <v>24</v>
@@ -9629,7 +10176,7 @@
       </c>
       <c r="I165" s="20"/>
     </row>
-    <row r="166" spans="1:9" ht="15">
+    <row r="166" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="20"/>
       <c r="B166" s="20" t="s">
         <v>24</v>
@@ -9652,7 +10199,7 @@
       </c>
       <c r="I166" s="20"/>
     </row>
-    <row r="167" spans="1:9" ht="15">
+    <row r="167" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="20" t="b">
         <v>0</v>
       </c>
@@ -9671,7 +10218,7 @@
       <c r="H167" s="20"/>
       <c r="I167" s="20"/>
     </row>
-    <row r="168" spans="1:9" ht="15">
+    <row r="168" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="20"/>
       <c r="B168" s="20" t="s">
         <v>24</v>
@@ -9696,7 +10243,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15">
+    <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="20"/>
       <c r="B169" s="20" t="s">
         <v>24</v>
@@ -9719,7 +10266,7 @@
       </c>
       <c r="I169" s="20"/>
     </row>
-    <row r="170" spans="1:9" ht="15">
+    <row r="170" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="20"/>
       <c r="B170" s="20" t="s">
         <v>24</v>
@@ -9742,7 +10289,7 @@
       </c>
       <c r="I170" s="20"/>
     </row>
-    <row r="171" spans="1:9" ht="15">
+    <row r="171" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="20"/>
       <c r="B171" s="20" t="s">
         <v>24</v>
@@ -9765,7 +10312,7 @@
       </c>
       <c r="I171" s="20"/>
     </row>
-    <row r="172" spans="1:9" ht="15">
+    <row r="172" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="20"/>
       <c r="B172" s="20" t="s">
         <v>24</v>
@@ -9788,7 +10335,7 @@
       </c>
       <c r="I172" s="20"/>
     </row>
-    <row r="173" spans="1:9" ht="15">
+    <row r="173" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="20"/>
       <c r="B173" s="20" t="s">
         <v>24</v>
@@ -9811,7 +10358,7 @@
       </c>
       <c r="I173" s="20"/>
     </row>
-    <row r="174" spans="1:9" ht="15">
+    <row r="174" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="20"/>
       <c r="B174" s="20" t="s">
         <v>24</v>
@@ -9834,7 +10381,7 @@
       </c>
       <c r="I174" s="20"/>
     </row>
-    <row r="175" spans="1:9" ht="15">
+    <row r="175" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="20"/>
       <c r="B175" s="20" t="s">
         <v>24</v>
@@ -9857,7 +10404,7 @@
       </c>
       <c r="I175" s="20"/>
     </row>
-    <row r="176" spans="1:9" ht="15">
+    <row r="176" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="20"/>
       <c r="B176" s="20" t="s">
         <v>24</v>
@@ -9880,7 +10427,7 @@
       </c>
       <c r="I176" s="20"/>
     </row>
-    <row r="177" spans="1:9" ht="15">
+    <row r="177" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="20"/>
       <c r="B177" s="20" t="s">
         <v>24</v>
@@ -9903,7 +10450,7 @@
       </c>
       <c r="I177" s="20"/>
     </row>
-    <row r="178" spans="1:9" ht="15">
+    <row r="178" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" s="20" t="b">
         <v>0</v>
       </c>
@@ -9922,7 +10469,7 @@
       <c r="H178" s="20"/>
       <c r="I178" s="20"/>
     </row>
-    <row r="179" spans="1:9" ht="15">
+    <row r="179" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A179" s="20"/>
       <c r="B179" s="20" t="s">
         <v>24</v>
@@ -9945,7 +10492,7 @@
       </c>
       <c r="I179" s="20"/>
     </row>
-    <row r="180" spans="1:9" ht="15">
+    <row r="180" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" s="20"/>
       <c r="B180" s="20" t="s">
         <v>24</v>
@@ -9968,7 +10515,7 @@
       </c>
       <c r="I180" s="20"/>
     </row>
-    <row r="181" spans="1:9" ht="15">
+    <row r="181" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="20"/>
       <c r="B181" s="20" t="s">
         <v>24</v>
@@ -9991,7 +10538,7 @@
       </c>
       <c r="I181" s="20"/>
     </row>
-    <row r="182" spans="1:9" ht="15">
+    <row r="182" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" s="20"/>
       <c r="B182" s="20" t="s">
         <v>24</v>
@@ -10014,7 +10561,7 @@
       </c>
       <c r="I182" s="20"/>
     </row>
-    <row r="183" spans="1:9" ht="15">
+    <row r="183" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A183" s="20" t="b">
         <v>0</v>
       </c>
@@ -10033,7 +10580,7 @@
       <c r="H183" s="20"/>
       <c r="I183" s="20"/>
     </row>
-    <row r="184" spans="1:9" ht="15">
+    <row r="184" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" s="20"/>
       <c r="B184" s="20" t="s">
         <v>24</v>
@@ -10056,7 +10603,7 @@
       </c>
       <c r="I184" s="20"/>
     </row>
-    <row r="185" spans="1:9" ht="15">
+    <row r="185" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="20"/>
       <c r="B185" s="20" t="s">
         <v>24</v>
@@ -10079,7 +10626,7 @@
       </c>
       <c r="I185" s="20"/>
     </row>
-    <row r="186" spans="1:9" ht="15">
+    <row r="186" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" s="20"/>
       <c r="B186" s="20" t="s">
         <v>24</v>
@@ -10102,7 +10649,7 @@
       </c>
       <c r="I186" s="20"/>
     </row>
-    <row r="187" spans="1:9" ht="15">
+    <row r="187" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="20"/>
       <c r="B187" s="20" t="s">
         <v>24</v>
@@ -10125,7 +10672,7 @@
       </c>
       <c r="I187" s="20"/>
     </row>
-    <row r="188" spans="1:9" ht="15">
+    <row r="188" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A188" s="20" t="b">
         <v>0</v>
       </c>
@@ -10144,7 +10691,7 @@
       <c r="H188" s="20"/>
       <c r="I188" s="20"/>
     </row>
-    <row r="189" spans="1:9" ht="15">
+    <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" s="20"/>
       <c r="B189" s="20" t="s">
         <v>24</v>
@@ -10165,7 +10712,7 @@
       <c r="H189" s="20"/>
       <c r="I189" s="20"/>
     </row>
-    <row r="190" spans="1:9" ht="15">
+    <row r="190" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" s="20"/>
       <c r="B190" s="20" t="s">
         <v>24</v>
@@ -10188,7 +10735,7 @@
       </c>
       <c r="I190" s="20"/>
     </row>
-    <row r="191" spans="1:9" ht="15">
+    <row r="191" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="20" t="b">
         <v>0</v>
       </c>
@@ -10207,7 +10754,7 @@
       <c r="H191" s="20"/>
       <c r="I191" s="20"/>
     </row>
-    <row r="192" spans="1:9" ht="15">
+    <row r="192" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" s="20"/>
       <c r="B192" s="20" t="s">
         <v>24</v>
@@ -10230,7 +10777,7 @@
       </c>
       <c r="I192" s="20"/>
     </row>
-    <row r="193" spans="1:9" ht="15">
+    <row r="193" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" s="20"/>
       <c r="B193" s="20" t="s">
         <v>24</v>
@@ -10255,7 +10802,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15">
+    <row r="194" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A194" s="20"/>
       <c r="B194" s="20" t="s">
         <v>24</v>
@@ -10276,7 +10823,7 @@
       <c r="H194" s="20"/>
       <c r="I194" s="20"/>
     </row>
-    <row r="195" spans="1:9" ht="15">
+    <row r="195" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A195" s="20"/>
       <c r="B195" s="20" t="s">
         <v>24</v>
@@ -10301,7 +10848,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15">
+    <row r="196" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A196" s="20"/>
       <c r="B196" s="20" t="s">
         <v>24</v>
@@ -10326,7 +10873,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15">
+    <row r="197" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="20" t="b">
         <v>0</v>
       </c>
@@ -10345,7 +10892,7 @@
       <c r="H197" s="20"/>
       <c r="I197" s="20"/>
     </row>
-    <row r="198" spans="1:9" ht="15">
+    <row r="198" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A198" s="20"/>
       <c r="B198" s="20" t="s">
         <v>24</v>
@@ -10370,7 +10917,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15">
+    <row r="199" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" s="20"/>
       <c r="B199" s="20" t="s">
         <v>24</v>
@@ -10393,7 +10940,7 @@
       </c>
       <c r="I199" s="20"/>
     </row>
-    <row r="200" spans="1:9" ht="15">
+    <row r="200" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" s="20"/>
       <c r="B200" s="20" t="s">
         <v>24</v>
@@ -10416,7 +10963,7 @@
       </c>
       <c r="I200" s="20"/>
     </row>
-    <row r="201" spans="1:9" ht="15">
+    <row r="201" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A201" s="20"/>
       <c r="B201" s="20" t="s">
         <v>24</v>
@@ -10439,7 +10986,7 @@
       </c>
       <c r="I201" s="20"/>
     </row>
-    <row r="202" spans="1:9" ht="15">
+    <row r="202" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A202" s="20"/>
       <c r="B202" s="20" t="s">
         <v>24</v>
@@ -10462,7 +11009,7 @@
       </c>
       <c r="I202" s="20"/>
     </row>
-    <row r="203" spans="1:9" ht="15">
+    <row r="203" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" s="20"/>
       <c r="B203" s="20" t="s">
         <v>24</v>
@@ -10485,7 +11032,7 @@
       </c>
       <c r="I203" s="20"/>
     </row>
-    <row r="204" spans="1:9" ht="15">
+    <row r="204" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" s="20"/>
       <c r="B204" s="20" t="s">
         <v>24</v>
@@ -10508,7 +11055,7 @@
       </c>
       <c r="I204" s="20"/>
     </row>
-    <row r="205" spans="1:9" ht="15">
+    <row r="205" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A205" s="20"/>
       <c r="B205" s="20" t="s">
         <v>24</v>
@@ -10531,7 +11078,7 @@
       </c>
       <c r="I205" s="20"/>
     </row>
-    <row r="206" spans="1:9" ht="15">
+    <row r="206" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A206" s="20"/>
       <c r="B206" s="20" t="s">
         <v>24</v>
@@ -10554,7 +11101,7 @@
       </c>
       <c r="I206" s="20"/>
     </row>
-    <row r="207" spans="1:9" ht="15">
+    <row r="207" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A207" s="20" t="b">
         <v>0</v>
       </c>
@@ -10573,7 +11120,7 @@
       <c r="H207" s="20"/>
       <c r="I207" s="20"/>
     </row>
-    <row r="208" spans="1:9" ht="15">
+    <row r="208" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A208" s="20"/>
       <c r="B208" s="20" t="s">
         <v>24</v>
@@ -10598,7 +11145,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15">
+    <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A209" s="20"/>
       <c r="B209" s="20" t="s">
         <v>24</v>
@@ -10621,7 +11168,7 @@
       </c>
       <c r="I209" s="20"/>
     </row>
-    <row r="210" spans="1:9" ht="15">
+    <row r="210" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A210" s="20"/>
       <c r="B210" s="20" t="s">
         <v>24</v>
@@ -10644,7 +11191,7 @@
       </c>
       <c r="I210" s="20"/>
     </row>
-    <row r="211" spans="1:9" ht="15">
+    <row r="211" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A211" s="20"/>
       <c r="B211" s="20" t="s">
         <v>24</v>
@@ -10667,7 +11214,7 @@
       </c>
       <c r="I211" s="20"/>
     </row>
-    <row r="212" spans="1:9" ht="15">
+    <row r="212" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A212" s="20"/>
       <c r="B212" s="20" t="s">
         <v>24</v>
@@ -10690,7 +11237,7 @@
       </c>
       <c r="I212" s="20"/>
     </row>
-    <row r="213" spans="1:9" ht="15">
+    <row r="213" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A213" s="20"/>
       <c r="B213" s="20" t="s">
         <v>24</v>
@@ -10713,7 +11260,7 @@
       </c>
       <c r="I213" s="20"/>
     </row>
-    <row r="214" spans="1:9" ht="15">
+    <row r="214" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A214" s="20"/>
       <c r="B214" s="20" t="s">
         <v>24</v>
@@ -10736,7 +11283,7 @@
       </c>
       <c r="I214" s="20"/>
     </row>
-    <row r="215" spans="1:9" ht="15">
+    <row r="215" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A215" s="20"/>
       <c r="B215" s="20" t="s">
         <v>24</v>
@@ -10759,7 +11306,7 @@
       </c>
       <c r="I215" s="20"/>
     </row>
-    <row r="216" spans="1:9" ht="15">
+    <row r="216" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A216" s="20"/>
       <c r="B216" s="20" t="s">
         <v>24</v>
@@ -10782,7 +11329,7 @@
       </c>
       <c r="I216" s="20"/>
     </row>
-    <row r="217" spans="1:9" ht="15">
+    <row r="217" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A217" s="20" t="b">
         <v>0</v>
       </c>
@@ -10801,7 +11348,7 @@
       <c r="H217" s="20"/>
       <c r="I217" s="20"/>
     </row>
-    <row r="218" spans="1:9" ht="15">
+    <row r="218" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" s="20"/>
       <c r="B218" s="20" t="s">
         <v>24</v>
@@ -10822,7 +11369,7 @@
       <c r="H218" s="20"/>
       <c r="I218" s="20"/>
     </row>
-    <row r="219" spans="1:9" ht="15">
+    <row r="219" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="20"/>
       <c r="B219" s="20" t="s">
         <v>24</v>
@@ -10845,7 +11392,7 @@
       </c>
       <c r="I219" s="20"/>
     </row>
-    <row r="220" spans="1:9" ht="15">
+    <row r="220" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" s="20"/>
       <c r="B220" s="20" t="s">
         <v>24</v>
@@ -10868,7 +11415,7 @@
       </c>
       <c r="I220" s="20"/>
     </row>
-    <row r="221" spans="1:9" ht="15">
+    <row r="221" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A221" s="20"/>
       <c r="B221" s="20" t="s">
         <v>24</v>
@@ -10891,7 +11438,7 @@
       </c>
       <c r="I221" s="20"/>
     </row>
-    <row r="222" spans="1:9" ht="15">
+    <row r="222" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" s="20"/>
       <c r="B222" s="20" t="s">
         <v>24</v>
@@ -10914,7 +11461,7 @@
       </c>
       <c r="I222" s="20"/>
     </row>
-    <row r="223" spans="1:9" ht="15">
+    <row r="223" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A223" s="20"/>
       <c r="B223" s="20" t="s">
         <v>24</v>
@@ -10937,7 +11484,7 @@
       </c>
       <c r="I223" s="20"/>
     </row>
-    <row r="224" spans="1:9" ht="15">
+    <row r="224" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" s="20"/>
       <c r="B224" s="20" t="s">
         <v>24</v>
@@ -10960,7 +11507,7 @@
       </c>
       <c r="I224" s="20"/>
     </row>
-    <row r="225" spans="1:9" ht="15">
+    <row r="225" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A225" s="20"/>
       <c r="B225" s="20" t="s">
         <v>24</v>
@@ -10983,7 +11530,7 @@
       </c>
       <c r="I225" s="20"/>
     </row>
-    <row r="226" spans="1:9" ht="15">
+    <row r="226" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A226" s="20"/>
       <c r="B226" s="20" t="s">
         <v>24</v>
@@ -11006,7 +11553,7 @@
       </c>
       <c r="I226" s="20"/>
     </row>
-    <row r="227" spans="1:9" ht="15">
+    <row r="227" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A227" s="20"/>
       <c r="B227" s="20" t="s">
         <v>24</v>
@@ -11029,7 +11576,7 @@
       </c>
       <c r="I227" s="20"/>
     </row>
-    <row r="228" spans="1:9" ht="15">
+    <row r="228" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A228" s="20"/>
       <c r="B228" s="20" t="s">
         <v>24</v>
@@ -11052,7 +11599,7 @@
       </c>
       <c r="I228" s="20"/>
     </row>
-    <row r="229" spans="1:9" ht="15">
+    <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="20"/>
       <c r="B229" s="20" t="s">
         <v>24</v>
@@ -11075,7 +11622,7 @@
       </c>
       <c r="I229" s="20"/>
     </row>
-    <row r="230" spans="1:9" ht="15">
+    <row r="230" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A230" s="20"/>
       <c r="B230" s="20" t="s">
         <v>24</v>
@@ -11098,7 +11645,7 @@
       </c>
       <c r="I230" s="20"/>
     </row>
-    <row r="231" spans="1:9" ht="15">
+    <row r="231" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A231" s="20"/>
       <c r="B231" s="20" t="s">
         <v>24</v>
@@ -11121,7 +11668,7 @@
       </c>
       <c r="I231" s="20"/>
     </row>
-    <row r="232" spans="1:9" ht="15">
+    <row r="232" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="20"/>
       <c r="B232" s="20" t="s">
         <v>24</v>
@@ -11144,7 +11691,7 @@
       </c>
       <c r="I232" s="20"/>
     </row>
-    <row r="233" spans="1:9" ht="15">
+    <row r="233" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="20"/>
       <c r="B233" s="20" t="s">
         <v>24</v>
@@ -11167,7 +11714,7 @@
       </c>
       <c r="I233" s="20"/>
     </row>
-    <row r="234" spans="1:9" ht="15">
+    <row r="234" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="20" t="b">
         <v>0</v>
       </c>
@@ -11186,7 +11733,7 @@
       <c r="H234" s="20"/>
       <c r="I234" s="20"/>
     </row>
-    <row r="235" spans="1:9" ht="15">
+    <row r="235" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A235" s="20"/>
       <c r="B235" s="20" t="s">
         <v>24</v>
@@ -11207,7 +11754,7 @@
       <c r="H235" s="20"/>
       <c r="I235" s="20"/>
     </row>
-    <row r="236" spans="1:9" ht="15">
+    <row r="236" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A236" s="20"/>
       <c r="B236" s="20" t="s">
         <v>24</v>
@@ -11230,7 +11777,7 @@
       </c>
       <c r="I236" s="20"/>
     </row>
-    <row r="237" spans="1:9" ht="15">
+    <row r="237" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A237" s="20"/>
       <c r="B237" s="20" t="s">
         <v>24</v>
@@ -11253,7 +11800,7 @@
       </c>
       <c r="I237" s="20"/>
     </row>
-    <row r="238" spans="1:9" ht="15">
+    <row r="238" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A238" s="20"/>
       <c r="B238" s="20" t="s">
         <v>24</v>
@@ -11276,7 +11823,7 @@
       </c>
       <c r="I238" s="20"/>
     </row>
-    <row r="239" spans="1:9" ht="15">
+    <row r="239" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A239" s="20"/>
       <c r="B239" s="20" t="s">
         <v>24</v>
@@ -11299,7 +11846,7 @@
       </c>
       <c r="I239" s="20"/>
     </row>
-    <row r="240" spans="1:9" ht="15">
+    <row r="240" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A240" s="20"/>
       <c r="B240" s="20" t="s">
         <v>24</v>
@@ -11322,7 +11869,7 @@
       </c>
       <c r="I240" s="20"/>
     </row>
-    <row r="241" spans="1:9" ht="15">
+    <row r="241" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A241" s="20"/>
       <c r="B241" s="20" t="s">
         <v>24</v>
@@ -11345,7 +11892,7 @@
       </c>
       <c r="I241" s="20"/>
     </row>
-    <row r="242" spans="1:9" ht="15">
+    <row r="242" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A242" s="20"/>
       <c r="B242" s="20" t="s">
         <v>24</v>
@@ -11368,7 +11915,7 @@
       </c>
       <c r="I242" s="20"/>
     </row>
-    <row r="243" spans="1:9" ht="15">
+    <row r="243" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A243" s="20"/>
       <c r="B243" s="20" t="s">
         <v>24</v>
@@ -11391,7 +11938,7 @@
       </c>
       <c r="I243" s="20"/>
     </row>
-    <row r="244" spans="1:9" ht="15">
+    <row r="244" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A244" s="20"/>
       <c r="B244" s="20" t="s">
         <v>24</v>
@@ -11414,7 +11961,7 @@
       </c>
       <c r="I244" s="20"/>
     </row>
-    <row r="245" spans="1:9" ht="15">
+    <row r="245" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A245" s="20"/>
       <c r="B245" s="20" t="s">
         <v>24</v>
@@ -11437,7 +11984,7 @@
       </c>
       <c r="I245" s="20"/>
     </row>
-    <row r="246" spans="1:9" ht="15">
+    <row r="246" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A246" s="20"/>
       <c r="B246" s="20" t="s">
         <v>24</v>
@@ -11460,7 +12007,7 @@
       </c>
       <c r="I246" s="20"/>
     </row>
-    <row r="247" spans="1:9" ht="15">
+    <row r="247" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A247" s="20"/>
       <c r="B247" s="20" t="s">
         <v>24</v>
@@ -11483,7 +12030,7 @@
       </c>
       <c r="I247" s="20"/>
     </row>
-    <row r="248" spans="1:9" ht="15">
+    <row r="248" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A248" s="20"/>
       <c r="B248" s="20" t="s">
         <v>24</v>
@@ -11506,7 +12053,7 @@
       </c>
       <c r="I248" s="20"/>
     </row>
-    <row r="249" spans="1:9" ht="15">
+    <row r="249" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A249" s="20"/>
       <c r="B249" s="20" t="s">
         <v>24</v>
@@ -11529,7 +12076,7 @@
       </c>
       <c r="I249" s="20"/>
     </row>
-    <row r="250" spans="1:9" ht="15">
+    <row r="250" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A250" s="20"/>
       <c r="B250" s="20" t="s">
         <v>24</v>
@@ -11552,7 +12099,7 @@
       </c>
       <c r="I250" s="20"/>
     </row>
-    <row r="251" spans="1:9" ht="15">
+    <row r="251" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A251" s="20" t="b">
         <v>0</v>
       </c>
@@ -11571,7 +12118,7 @@
       <c r="H251" s="20"/>
       <c r="I251" s="20"/>
     </row>
-    <row r="252" spans="1:9" ht="15">
+    <row r="252" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A252" s="20"/>
       <c r="B252" s="20" t="s">
         <v>24</v>
@@ -11596,7 +12143,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15">
+    <row r="253" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A253" s="20"/>
       <c r="B253" s="20" t="s">
         <v>24</v>
@@ -11619,7 +12166,7 @@
       </c>
       <c r="I253" s="20"/>
     </row>
-    <row r="254" spans="1:9" ht="15">
+    <row r="254" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A254" s="20"/>
       <c r="B254" s="20" t="s">
         <v>24</v>
@@ -11642,7 +12189,7 @@
       </c>
       <c r="I254" s="20"/>
     </row>
-    <row r="255" spans="1:9" ht="15">
+    <row r="255" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A255" s="20"/>
       <c r="B255" s="20" t="s">
         <v>24</v>
@@ -11665,7 +12212,7 @@
       </c>
       <c r="I255" s="20"/>
     </row>
-    <row r="256" spans="1:9" ht="15">
+    <row r="256" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A256" s="20"/>
       <c r="B256" s="20" t="s">
         <v>24</v>
@@ -11688,7 +12235,7 @@
       </c>
       <c r="I256" s="20"/>
     </row>
-    <row r="257" spans="1:9" ht="15">
+    <row r="257" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A257" s="20" t="b">
         <v>0</v>
       </c>
@@ -11707,7 +12254,7 @@
       <c r="H257" s="20"/>
       <c r="I257" s="20"/>
     </row>
-    <row r="258" spans="1:9" ht="15">
+    <row r="258" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A258" s="20"/>
       <c r="B258" s="20" t="s">
         <v>24</v>
@@ -11732,7 +12279,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15">
+    <row r="259" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A259" s="20"/>
       <c r="B259" s="20" t="s">
         <v>24</v>
@@ -11755,7 +12302,7 @@
       </c>
       <c r="I259" s="20"/>
     </row>
-    <row r="260" spans="1:9" ht="15">
+    <row r="260" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A260" s="20" t="b">
         <v>0</v>
       </c>
@@ -11774,7 +12321,7 @@
       <c r="H260" s="20"/>
       <c r="I260" s="20"/>
     </row>
-    <row r="261" spans="1:9" ht="15">
+    <row r="261" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A261" s="20" t="b">
         <v>0</v>
       </c>
@@ -11793,7 +12340,7 @@
       <c r="H261" s="20"/>
       <c r="I261" s="20"/>
     </row>
-    <row r="262" spans="1:9" ht="15">
+    <row r="262" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A262" s="20" t="b">
         <v>0</v>
       </c>
@@ -11812,7 +12359,7 @@
       <c r="H262" s="20"/>
       <c r="I262" s="20"/>
     </row>
-    <row r="263" spans="1:9" ht="15">
+    <row r="263" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A263" s="20"/>
       <c r="B263" s="20" t="s">
         <v>24</v>
@@ -11833,7 +12380,7 @@
       <c r="H263" s="20"/>
       <c r="I263" s="20"/>
     </row>
-    <row r="264" spans="1:9" ht="15">
+    <row r="264" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A264" s="20"/>
       <c r="B264" s="20" t="s">
         <v>24</v>
@@ -11856,7 +12403,7 @@
       </c>
       <c r="I264" s="20"/>
     </row>
-    <row r="265" spans="1:9" ht="15">
+    <row r="265" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A265" s="20"/>
       <c r="B265" s="20" t="s">
         <v>24</v>
@@ -11879,7 +12426,7 @@
       </c>
       <c r="I265" s="20"/>
     </row>
-    <row r="266" spans="1:9" ht="15">
+    <row r="266" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A266" s="20"/>
       <c r="B266" s="20" t="s">
         <v>24</v>
@@ -11902,7 +12449,7 @@
       </c>
       <c r="I266" s="20"/>
     </row>
-    <row r="267" spans="1:9" ht="15">
+    <row r="267" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A267" s="20"/>
       <c r="B267" s="20" t="s">
         <v>24</v>
@@ -11925,7 +12472,7 @@
       </c>
       <c r="I267" s="20"/>
     </row>
-    <row r="268" spans="1:9" ht="15">
+    <row r="268" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A268" s="20"/>
       <c r="B268" s="20" t="s">
         <v>24</v>
@@ -11948,7 +12495,7 @@
       </c>
       <c r="I268" s="20"/>
     </row>
-    <row r="269" spans="1:9" ht="15">
+    <row r="269" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A269" s="20"/>
       <c r="B269" s="20" t="s">
         <v>24</v>
@@ -11971,7 +12518,7 @@
       </c>
       <c r="I269" s="20"/>
     </row>
-    <row r="270" spans="1:9" ht="15">
+    <row r="270" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A270" s="20"/>
       <c r="B270" s="20" t="s">
         <v>24</v>
@@ -11994,7 +12541,7 @@
       </c>
       <c r="I270" s="20"/>
     </row>
-    <row r="271" spans="1:9" ht="15">
+    <row r="271" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A271" s="20"/>
       <c r="B271" s="20" t="s">
         <v>24</v>
@@ -12017,7 +12564,7 @@
       </c>
       <c r="I271" s="20"/>
     </row>
-    <row r="272" spans="1:9" ht="15">
+    <row r="272" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A272" s="20"/>
       <c r="B272" s="20" t="s">
         <v>24</v>
@@ -12040,7 +12587,7 @@
       </c>
       <c r="I272" s="20"/>
     </row>
-    <row r="273" spans="1:9" ht="15">
+    <row r="273" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A273" s="20"/>
       <c r="B273" s="20" t="s">
         <v>24</v>
@@ -12063,7 +12610,7 @@
       </c>
       <c r="I273" s="20"/>
     </row>
-    <row r="274" spans="1:9" ht="15">
+    <row r="274" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A274" s="20" t="b">
         <v>0</v>
       </c>
@@ -12082,7 +12629,7 @@
       <c r="H274" s="20"/>
       <c r="I274" s="20"/>
     </row>
-    <row r="275" spans="1:9" ht="15">
+    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A275" s="20"/>
       <c r="B275" s="20" t="s">
         <v>24</v>
@@ -12105,7 +12652,7 @@
       </c>
       <c r="I275" s="20"/>
     </row>
-    <row r="276" spans="1:9" ht="15">
+    <row r="276" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A276" s="20" t="b">
         <v>0</v>
       </c>
@@ -12124,7 +12671,7 @@
       <c r="H276" s="20"/>
       <c r="I276" s="20"/>
     </row>
-    <row r="277" spans="1:9" ht="15">
+    <row r="277" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A277" s="20"/>
       <c r="B277" s="20" t="s">
         <v>24</v>
@@ -12149,7 +12696,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15">
+    <row r="278" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A278" s="20"/>
       <c r="B278" s="20" t="s">
         <v>24</v>
@@ -12172,7 +12719,7 @@
       </c>
       <c r="I278" s="20"/>
     </row>
-    <row r="279" spans="1:9" ht="15">
+    <row r="279" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A279" s="20"/>
       <c r="B279" s="20" t="s">
         <v>24</v>
@@ -12195,7 +12742,7 @@
       </c>
       <c r="I279" s="20"/>
     </row>
-    <row r="280" spans="1:9" ht="15">
+    <row r="280" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A280" s="20"/>
       <c r="B280" s="20" t="s">
         <v>24</v>
@@ -12218,7 +12765,7 @@
       </c>
       <c r="I280" s="20"/>
     </row>
-    <row r="281" spans="1:9" ht="15">
+    <row r="281" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A281" s="20"/>
       <c r="B281" s="20" t="s">
         <v>24</v>
@@ -12241,7 +12788,7 @@
       </c>
       <c r="I281" s="20"/>
     </row>
-    <row r="282" spans="1:9" ht="15">
+    <row r="282" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A282" s="20"/>
       <c r="B282" s="20" t="s">
         <v>24</v>
@@ -12264,7 +12811,7 @@
       </c>
       <c r="I282" s="20"/>
     </row>
-    <row r="283" spans="1:9" ht="15">
+    <row r="283" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A283" s="20"/>
       <c r="B283" s="20" t="s">
         <v>24</v>
@@ -12287,7 +12834,7 @@
       </c>
       <c r="I283" s="20"/>
     </row>
-    <row r="284" spans="1:9" ht="15">
+    <row r="284" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A284" s="20"/>
       <c r="B284" s="20" t="s">
         <v>24</v>
@@ -12310,7 +12857,7 @@
       </c>
       <c r="I284" s="20"/>
     </row>
-    <row r="285" spans="1:9" ht="15">
+    <row r="285" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A285" s="20"/>
       <c r="B285" s="20" t="s">
         <v>24</v>
@@ -12333,7 +12880,7 @@
       </c>
       <c r="I285" s="20"/>
     </row>
-    <row r="286" spans="1:9" ht="15">
+    <row r="286" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A286" s="20"/>
       <c r="B286" s="20" t="s">
         <v>24</v>
@@ -12356,7 +12903,7 @@
       </c>
       <c r="I286" s="20"/>
     </row>
-    <row r="287" spans="1:9" ht="15">
+    <row r="287" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A287" s="20"/>
       <c r="B287" s="20" t="s">
         <v>24</v>
@@ -12379,7 +12926,7 @@
       </c>
       <c r="I287" s="20"/>
     </row>
-    <row r="288" spans="1:9" ht="15">
+    <row r="288" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A288" s="20" t="b">
         <v>0</v>
       </c>
@@ -12398,7 +12945,7 @@
       <c r="H288" s="20"/>
       <c r="I288" s="20"/>
     </row>
-    <row r="289" spans="1:9" ht="15">
+    <row r="289" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A289" s="20"/>
       <c r="B289" s="20" t="s">
         <v>24</v>
@@ -12421,7 +12968,7 @@
       </c>
       <c r="I289" s="20"/>
     </row>
-    <row r="290" spans="1:9" ht="15">
+    <row r="290" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A290" s="20" t="b">
         <v>0</v>
       </c>
@@ -12440,7 +12987,7 @@
       <c r="H290" s="20"/>
       <c r="I290" s="20"/>
     </row>
-    <row r="291" spans="1:9" ht="15">
+    <row r="291" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A291" s="20"/>
       <c r="B291" s="20" t="s">
         <v>24</v>
@@ -12461,7 +13008,7 @@
       <c r="H291" s="20"/>
       <c r="I291" s="20"/>
     </row>
-    <row r="292" spans="1:9" ht="15">
+    <row r="292" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A292" s="20" t="b">
         <v>0</v>
       </c>
@@ -12480,7 +13027,7 @@
       <c r="H292" s="20"/>
       <c r="I292" s="20"/>
     </row>
-    <row r="293" spans="1:9" ht="15">
+    <row r="293" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A293" s="20"/>
       <c r="B293" s="20" t="s">
         <v>24</v>
@@ -12501,7 +13048,7 @@
       <c r="H293" s="20"/>
       <c r="I293" s="20"/>
     </row>
-    <row r="294" spans="1:9" ht="15">
+    <row r="294" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A294" s="20" t="b">
         <v>0</v>
       </c>
@@ -12520,7 +13067,7 @@
       <c r="H294" s="20"/>
       <c r="I294" s="20"/>
     </row>
-    <row r="295" spans="1:9" ht="15">
+    <row r="295" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A295" s="20"/>
       <c r="B295" s="20" t="s">
         <v>24</v>
@@ -12541,7 +13088,7 @@
       <c r="H295" s="20"/>
       <c r="I295" s="20"/>
     </row>
-    <row r="296" spans="1:9" ht="15">
+    <row r="296" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A296" s="20" t="b">
         <v>0</v>
       </c>
@@ -12560,7 +13107,7 @@
       <c r="H296" s="20"/>
       <c r="I296" s="20"/>
     </row>
-    <row r="297" spans="1:9" ht="15">
+    <row r="297" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A297" s="20"/>
       <c r="B297" s="20" t="s">
         <v>24</v>
@@ -12583,7 +13130,7 @@
       </c>
       <c r="I297" s="20"/>
     </row>
-    <row r="298" spans="1:9" ht="15">
+    <row r="298" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A298" s="20" t="b">
         <v>0</v>
       </c>
@@ -12602,7 +13149,7 @@
       <c r="H298" s="20"/>
       <c r="I298" s="20"/>
     </row>
-    <row r="299" spans="1:9" ht="15">
+    <row r="299" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A299" s="20"/>
       <c r="B299" s="20" t="s">
         <v>24</v>
@@ -12627,7 +13174,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15">
+    <row r="300" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A300" s="20"/>
       <c r="B300" s="20" t="s">
         <v>24</v>
@@ -12650,7 +13197,7 @@
       </c>
       <c r="I300" s="20"/>
     </row>
-    <row r="301" spans="1:9" ht="15">
+    <row r="301" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A301" s="20"/>
       <c r="B301" s="20" t="s">
         <v>24</v>
@@ -12673,7 +13220,7 @@
       </c>
       <c r="I301" s="20"/>
     </row>
-    <row r="302" spans="1:9" ht="15">
+    <row r="302" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A302" s="20"/>
       <c r="B302" s="20" t="s">
         <v>24</v>
@@ -12696,7 +13243,7 @@
       </c>
       <c r="I302" s="20"/>
     </row>
-    <row r="303" spans="1:9" ht="15">
+    <row r="303" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A303" s="20"/>
       <c r="B303" s="20" t="s">
         <v>24</v>
@@ -12719,7 +13266,7 @@
       </c>
       <c r="I303" s="20"/>
     </row>
-    <row r="304" spans="1:9" ht="15">
+    <row r="304" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A304" s="20"/>
       <c r="B304" s="20" t="s">
         <v>24</v>
@@ -12742,7 +13289,7 @@
       </c>
       <c r="I304" s="20"/>
     </row>
-    <row r="305" spans="1:9" ht="15">
+    <row r="305" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A305" s="20"/>
       <c r="B305" s="20" t="s">
         <v>24</v>
@@ -12765,7 +13312,7 @@
       </c>
       <c r="I305" s="20"/>
     </row>
-    <row r="306" spans="1:9" ht="15">
+    <row r="306" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A306" s="20"/>
       <c r="B306" s="20" t="s">
         <v>24</v>
@@ -12788,7 +13335,7 @@
       </c>
       <c r="I306" s="20"/>
     </row>
-    <row r="307" spans="1:9" ht="15">
+    <row r="307" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A307" s="20"/>
       <c r="B307" s="20" t="s">
         <v>24</v>
@@ -12811,7 +13358,7 @@
       </c>
       <c r="I307" s="20"/>
     </row>
-    <row r="308" spans="1:9" ht="15">
+    <row r="308" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A308" s="20" t="b">
         <v>0</v>
       </c>
@@ -12830,7 +13377,7 @@
       <c r="H308" s="20"/>
       <c r="I308" s="20"/>
     </row>
-    <row r="309" spans="1:9" ht="15">
+    <row r="309" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A309" s="20"/>
       <c r="B309" s="20" t="s">
         <v>24</v>
@@ -12853,7 +13400,7 @@
       </c>
       <c r="I309" s="20"/>
     </row>
-    <row r="310" spans="1:9" ht="15">
+    <row r="310" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A310" s="20"/>
       <c r="B310" s="20" t="s">
         <v>24</v>
@@ -12876,7 +13423,7 @@
       </c>
       <c r="I310" s="20"/>
     </row>
-    <row r="311" spans="1:9" ht="15">
+    <row r="311" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A311" s="20"/>
       <c r="B311" s="20" t="s">
         <v>24</v>
@@ -12899,7 +13446,7 @@
       </c>
       <c r="I311" s="20"/>
     </row>
-    <row r="312" spans="1:9" ht="15">
+    <row r="312" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A312" s="20"/>
       <c r="B312" s="20" t="s">
         <v>24</v>
@@ -12922,7 +13469,7 @@
       </c>
       <c r="I312" s="20"/>
     </row>
-    <row r="313" spans="1:9" ht="15">
+    <row r="313" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A313" s="20" t="b">
         <v>0</v>
       </c>
@@ -12941,7 +13488,7 @@
       <c r="H313" s="20"/>
       <c r="I313" s="20"/>
     </row>
-    <row r="314" spans="1:9" ht="15">
+    <row r="314" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A314" s="20"/>
       <c r="B314" s="20" t="s">
         <v>24</v>
@@ -12964,7 +13511,7 @@
       </c>
       <c r="I314" s="20"/>
     </row>
-    <row r="315" spans="1:9" ht="15">
+    <row r="315" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A315" s="20"/>
       <c r="B315" s="20" t="s">
         <v>24</v>
@@ -12987,7 +13534,7 @@
       </c>
       <c r="I315" s="20"/>
     </row>
-    <row r="316" spans="1:9" ht="15">
+    <row r="316" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A316" s="20"/>
       <c r="B316" s="20" t="s">
         <v>24</v>
@@ -13012,7 +13559,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15">
+    <row r="317" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A317" s="20" t="b">
         <v>0</v>
       </c>
@@ -13031,7 +13578,7 @@
       <c r="H317" s="20"/>
       <c r="I317" s="20"/>
     </row>
-    <row r="318" spans="1:9" ht="15">
+    <row r="318" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A318" s="20"/>
       <c r="B318" s="20" t="s">
         <v>24</v>
@@ -13056,7 +13603,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15">
+    <row r="319" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A319" s="20"/>
       <c r="B319" s="20" t="s">
         <v>24</v>
@@ -13079,7 +13626,7 @@
       </c>
       <c r="I319" s="20"/>
     </row>
-    <row r="320" spans="1:9" ht="15">
+    <row r="320" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A320" s="20" t="b">
         <v>0</v>
       </c>
@@ -13098,7 +13645,7 @@
       <c r="H320" s="20"/>
       <c r="I320" s="20"/>
     </row>
-    <row r="321" spans="1:9" ht="15">
+    <row r="321" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A321" s="20"/>
       <c r="B321" s="20" t="s">
         <v>24</v>
@@ -13119,7 +13666,7 @@
       <c r="H321" s="20"/>
       <c r="I321" s="20"/>
     </row>
-    <row r="322" spans="1:9" ht="15">
+    <row r="322" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A322" s="20"/>
       <c r="B322" s="20" t="s">
         <v>24</v>
@@ -13140,7 +13687,7 @@
       <c r="H322" s="20"/>
       <c r="I322" s="20"/>
     </row>
-    <row r="323" spans="1:9" ht="15">
+    <row r="323" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A323" s="20"/>
       <c r="B323" s="20" t="s">
         <v>24</v>
@@ -13163,7 +13710,7 @@
       </c>
       <c r="I323" s="20"/>
     </row>
-    <row r="324" spans="1:9" ht="15">
+    <row r="324" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A324" s="20" t="b">
         <v>0</v>
       </c>
@@ -13182,7 +13729,7 @@
       <c r="H324" s="20"/>
       <c r="I324" s="20"/>
     </row>
-    <row r="325" spans="1:9" ht="15">
+    <row r="325" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A325" s="20" t="b">
         <v>0</v>
       </c>
@@ -13201,7 +13748,7 @@
       <c r="H325" s="20"/>
       <c r="I325" s="20"/>
     </row>
-    <row r="326" spans="1:9" ht="15">
+    <row r="326" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A326" s="20"/>
       <c r="B326" s="20" t="s">
         <v>24</v>
@@ -13226,7 +13773,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15">
+    <row r="327" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A327" s="20"/>
       <c r="B327" s="20" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
add back in the discrete variables in the test spreadsheets
</commit_message>
<xml_diff>
--- a/spec/files/discrete_variables.xlsx
+++ b/spec/files/discrete_variables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12816" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$Y$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Y$13</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1621,8 +1621,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1241">
+  <cellStyleXfs count="1247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2930,7 +2936,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1241">
+  <cellStyles count="1247">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3551,6 +3557,9 @@
     <cellStyle name="Followed Hyperlink" xfId="1236" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1246" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4171,6 +4180,9 @@
     <cellStyle name="Hyperlink" xfId="1235" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1245" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4184,21 +4196,23 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instructions"/>
       <sheetName val="Setup"/>
       <sheetName val="Variables"/>
+      <sheetName val="Outputs"/>
       <sheetName val="BCL Measure Data"/>
       <sheetName val="Lookups"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5">
         <row r="2">
           <cell r="A2" t="str">
             <v>m2.xlarge</v>
@@ -4542,17 +4556,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="50.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -4576,17 +4590,17 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.77734375" style="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="21"/>
@@ -4595,7 +4609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="13" customFormat="1">
       <c r="A2" s="12" t="s">
         <v>451</v>
       </c>
@@ -4604,7 +4618,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>452</v>
       </c>
@@ -4615,7 +4629,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>454</v>
       </c>
@@ -4634,7 +4648,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28">
       <c r="A5" s="1" t="s">
         <v>457</v>
       </c>
@@ -4653,7 +4667,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="13" customFormat="1">
       <c r="A7" s="12" t="s">
         <v>32</v>
       </c>
@@ -4662,7 +4676,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -4673,7 +4687,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -4681,7 +4695,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -4689,7 +4703,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A12" s="12" t="s">
         <v>31</v>
       </c>
@@ -4700,7 +4714,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>462</v>
       </c>
@@ -4708,7 +4722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A15" s="12" t="s">
         <v>463</v>
       </c>
@@ -4719,7 +4733,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -4727,7 +4741,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -4735,7 +4749,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>465</v>
       </c>
@@ -4744,7 +4758,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A20" s="12" t="s">
         <v>38</v>
       </c>
@@ -4757,7 +4771,7 @@
       <c r="D20" s="12"/>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -4765,7 +4779,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A23" s="12" t="s">
         <v>34</v>
       </c>
@@ -4782,7 +4796,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="28">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
@@ -4799,7 +4813,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A26" s="12" t="s">
         <v>40</v>
       </c>
@@ -4843,34 +4857,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="5"/>
-    <col min="10" max="13" width="11.44140625" style="1"/>
+    <col min="9" max="9" width="11.5" style="5"/>
+    <col min="10" max="13" width="11.5" style="1"/>
     <col min="14" max="14" width="13.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.77734375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" style="1"/>
-    <col min="18" max="18" width="46.109375" style="1" customWidth="1"/>
-    <col min="19" max="21" width="11.44140625" style="1"/>
+    <col min="16" max="16" width="16.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="1"/>
+    <col min="18" max="18" width="46.1640625" style="1" customWidth="1"/>
+    <col min="19" max="21" width="11.5" style="1"/>
     <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="1"/>
+    <col min="23" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="18">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -4904,7 +4918,7 @@
       <c r="W1" s="29"/>
       <c r="X1" s="29"/>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -4917,7 +4931,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:24" s="16" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="16" customFormat="1" ht="45">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -4988,7 +5002,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -5014,7 +5028,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>24</v>
@@ -5047,7 +5061,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6"/>
       <c r="B6" t="s">
         <v>25</v>
@@ -5086,7 +5100,7 @@
       </c>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7"/>
       <c r="B7" t="s">
         <v>24</v>
@@ -5116,7 +5130,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24">
       <c r="A8"/>
       <c r="B8" t="s">
         <v>24</v>
@@ -5146,7 +5160,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24">
       <c r="A9"/>
       <c r="B9" t="s">
         <v>24</v>
@@ -5176,7 +5190,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24">
       <c r="A10"/>
       <c r="B10" t="s">
         <v>24</v>
@@ -5208,7 +5222,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24">
       <c r="A11"/>
       <c r="B11" t="s">
         <v>24</v>
@@ -5238,7 +5252,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24">
       <c r="A12"/>
       <c r="B12" t="s">
         <v>24</v>
@@ -5268,7 +5282,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24">
       <c r="A13"/>
       <c r="B13" t="s">
         <v>24</v>
@@ -5298,7 +5312,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" customFormat="1">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -5312,7 +5326,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" customFormat="1">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -5335,7 +5349,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" customFormat="1">
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -5373,7 +5387,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" customFormat="1">
       <c r="B17" t="s">
         <v>24</v>
       </c>
@@ -5393,7 +5407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" customFormat="1">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -5413,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" customFormat="1">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -5433,7 +5447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" customFormat="1" ht="15">
       <c r="A20" s="20" t="b">
         <v>1</v>
       </c>
@@ -5459,7 +5473,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" customFormat="1" ht="15">
       <c r="A21" s="20"/>
       <c r="B21" s="20" t="s">
         <v>25</v>
@@ -5500,7 +5514,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" customFormat="1" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>25</v>
@@ -5541,7 +5555,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" customFormat="1" ht="15">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>25</v>
@@ -5573,7 +5587,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="24" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" customFormat="1" ht="15">
       <c r="A24" s="20" t="b">
         <v>1</v>
       </c>
@@ -5592,7 +5606,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" customFormat="1" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>25</v>
@@ -5633,7 +5647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" customFormat="1" ht="15">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>24</v>
@@ -5656,7 +5670,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" customFormat="1" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>24</v>
@@ -5679,7 +5693,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" customFormat="1" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>24</v>
@@ -5702,7 +5716,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" customFormat="1" ht="15">
       <c r="A29" s="20" t="b">
         <v>1</v>
       </c>
@@ -5721,7 +5735,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" customFormat="1" ht="15">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>25</v>
@@ -5762,7 +5776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" customFormat="1" ht="15">
       <c r="A31" s="20"/>
       <c r="B31" s="20" t="s">
         <v>24</v>
@@ -5785,7 +5799,7 @@
       </c>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" customFormat="1" ht="15">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>24</v>
@@ -5808,7 +5822,7 @@
       </c>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" customFormat="1" ht="15">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>24</v>
@@ -5831,7 +5845,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" customFormat="1" ht="15">
       <c r="A34" s="20" t="b">
         <v>1</v>
       </c>
@@ -5850,7 +5864,7 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" customFormat="1" ht="15">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>24</v>
@@ -5875,7 +5889,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" customFormat="1" ht="15">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>25</v>
@@ -5923,34 +5937,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E2"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="5"/>
-    <col min="10" max="13" width="11.44140625" style="1"/>
+    <col min="9" max="9" width="11.5" style="5"/>
+    <col min="10" max="13" width="11.5" style="1"/>
     <col min="14" max="14" width="13.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.77734375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" style="1"/>
-    <col min="18" max="18" width="46.109375" style="1" customWidth="1"/>
-    <col min="19" max="21" width="11.44140625" style="1"/>
+    <col min="16" max="16" width="16.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="1"/>
+    <col min="18" max="18" width="46.1640625" style="1" customWidth="1"/>
+    <col min="19" max="21" width="11.5" style="1"/>
     <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="1"/>
+    <col min="23" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="18">
       <c r="A1" s="9" t="s">
         <v>482</v>
       </c>
@@ -5986,7 +6000,7 @@
       <c r="W1" s="29"/>
       <c r="X1" s="29"/>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15">
       <c r="A2" s="16"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5999,7 +6013,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:24" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="16" customFormat="1" ht="15">
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -6019,7 +6033,7 @@
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -6036,7 +6050,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -6055,7 +6069,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -6073,7 +6087,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="15"/>
@@ -6091,7 +6105,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -6109,7 +6123,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -6127,7 +6141,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -6145,7 +6159,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -6163,7 +6177,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -6181,7 +6195,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -6199,9 +6213,9 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:24" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:24" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" customFormat="1"/>
+    <row r="15" spans="1:24" customFormat="1"/>
+    <row r="16" spans="1:24" customFormat="1">
       <c r="C16" s="19"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -6211,10 +6225,10 @@
       <c r="O16" s="3"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" customFormat="1"/>
+    <row r="18" spans="1:16" customFormat="1"/>
+    <row r="19" spans="1:16" customFormat="1"/>
+    <row r="20" spans="1:16" customFormat="1" ht="15">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -6232,7 +6246,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" customFormat="1" ht="15">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -6250,7 +6264,7 @@
       <c r="O21" s="3"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" customFormat="1" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -6268,7 +6282,7 @@
       <c r="O22" s="3"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" customFormat="1" ht="15">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -6279,7 +6293,7 @@
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" customFormat="1" ht="15">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -6290,7 +6304,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" customFormat="1" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -6306,7 +6320,7 @@
       <c r="O25" s="3"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" customFormat="1" ht="15">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -6317,7 +6331,7 @@
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" customFormat="1" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -6328,7 +6342,7 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" customFormat="1" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -6339,7 +6353,7 @@
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" customFormat="1" ht="15">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
@@ -6350,7 +6364,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" customFormat="1" ht="15">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
@@ -6366,7 +6380,7 @@
       <c r="O30" s="3"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" customFormat="1" ht="15">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
@@ -6377,7 +6391,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" customFormat="1" ht="15">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -6388,7 +6402,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" customFormat="1" ht="15">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
@@ -6399,7 +6413,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" customFormat="1" ht="15">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
@@ -6410,7 +6424,7 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" customFormat="1" ht="15">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -6421,7 +6435,7 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" customFormat="1" ht="15">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -6440,6 +6454,11 @@
   <autoFilter ref="A2:Y13"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6451,19 +6470,19 @@
       <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="20" t="b">
         <v>0</v>
       </c>
@@ -6482,7 +6501,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
         <v>24</v>
@@ -6503,7 +6522,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
         <v>24</v>
@@ -6526,7 +6545,7 @@
       </c>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="20"/>
       <c r="B4" s="20" t="s">
         <v>24</v>
@@ -6549,7 +6568,7 @@
       </c>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="20"/>
       <c r="B5" s="20" t="s">
         <v>24</v>
@@ -6572,7 +6591,7 @@
       </c>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="20"/>
       <c r="B6" s="20" t="s">
         <v>24</v>
@@ -6595,7 +6614,7 @@
       </c>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="20"/>
       <c r="B7" s="20" t="s">
         <v>24</v>
@@ -6618,7 +6637,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="20"/>
       <c r="B8" s="20" t="s">
         <v>24</v>
@@ -6641,7 +6660,7 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="20"/>
       <c r="B9" s="20" t="s">
         <v>24</v>
@@ -6664,7 +6683,7 @@
       </c>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
         <v>24</v>
@@ -6687,7 +6706,7 @@
       </c>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" s="20" t="b">
         <v>0</v>
       </c>
@@ -6706,7 +6725,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" s="20"/>
       <c r="B12" s="20" t="s">
         <v>24</v>
@@ -6727,7 +6746,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15">
       <c r="A13" s="20"/>
       <c r="B13" s="20" t="s">
         <v>24</v>
@@ -6750,7 +6769,7 @@
       </c>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" s="20"/>
       <c r="B14" s="20" t="s">
         <v>24</v>
@@ -6773,7 +6792,7 @@
       </c>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15">
       <c r="A15" s="20"/>
       <c r="B15" s="20" t="s">
         <v>24</v>
@@ -6796,7 +6815,7 @@
       </c>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15">
       <c r="A16" s="20"/>
       <c r="B16" s="20" t="s">
         <v>24</v>
@@ -6819,7 +6838,7 @@
       </c>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15">
       <c r="A17" s="20"/>
       <c r="B17" s="20" t="s">
         <v>24</v>
@@ -6842,7 +6861,7 @@
       </c>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15">
       <c r="A18" s="20"/>
       <c r="B18" s="20" t="s">
         <v>24</v>
@@ -6865,7 +6884,7 @@
       </c>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15">
       <c r="A19" s="20"/>
       <c r="B19" s="20" t="s">
         <v>24</v>
@@ -6888,7 +6907,7 @@
       </c>
       <c r="I19" s="20"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
         <v>24</v>
@@ -6911,7 +6930,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15">
       <c r="A21" s="20" t="b">
         <v>0</v>
       </c>
@@ -6930,7 +6949,7 @@
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>24</v>
@@ -6953,7 +6972,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>24</v>
@@ -6976,7 +6995,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15">
       <c r="A24" s="20"/>
       <c r="B24" s="20" t="s">
         <v>24</v>
@@ -6999,7 +7018,7 @@
       </c>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>24</v>
@@ -7022,7 +7041,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>24</v>
@@ -7045,7 +7064,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>24</v>
@@ -7068,7 +7087,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>24</v>
@@ -7091,7 +7110,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15">
       <c r="A29" s="20"/>
       <c r="B29" s="20" t="s">
         <v>24</v>
@@ -7114,7 +7133,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>24</v>
@@ -7137,7 +7156,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15">
       <c r="A31" s="20" t="b">
         <v>0</v>
       </c>
@@ -7156,7 +7175,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>24</v>
@@ -7177,7 +7196,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>24</v>
@@ -7200,7 +7219,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15">
       <c r="A34" s="20"/>
       <c r="B34" s="20" t="s">
         <v>24</v>
@@ -7223,7 +7242,7 @@
       </c>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>24</v>
@@ -7246,7 +7265,7 @@
       </c>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>24</v>
@@ -7269,7 +7288,7 @@
       </c>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15">
       <c r="A37" s="20"/>
       <c r="B37" s="20" t="s">
         <v>24</v>
@@ -7292,7 +7311,7 @@
       </c>
       <c r="I37" s="20"/>
     </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15">
       <c r="A38" s="20"/>
       <c r="B38" s="20" t="s">
         <v>24</v>
@@ -7315,7 +7334,7 @@
       </c>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15">
       <c r="A39" s="20"/>
       <c r="B39" s="20" t="s">
         <v>24</v>
@@ -7338,7 +7357,7 @@
       </c>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15">
       <c r="A40" s="20"/>
       <c r="B40" s="20" t="s">
         <v>24</v>
@@ -7361,7 +7380,7 @@
       </c>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15">
       <c r="A41" s="20" t="b">
         <v>0</v>
       </c>
@@ -7380,7 +7399,7 @@
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15">
       <c r="A42" s="20"/>
       <c r="B42" s="20" t="s">
         <v>24</v>
@@ -7401,7 +7420,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15">
       <c r="A43" s="20"/>
       <c r="B43" s="20" t="s">
         <v>24</v>
@@ -7424,7 +7443,7 @@
       </c>
       <c r="I43" s="20"/>
     </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15">
       <c r="A44" s="20"/>
       <c r="B44" s="20" t="s">
         <v>24</v>
@@ -7447,7 +7466,7 @@
       </c>
       <c r="I44" s="20"/>
     </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15">
       <c r="A45" s="20"/>
       <c r="B45" s="20" t="s">
         <v>24</v>
@@ -7470,7 +7489,7 @@
       </c>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15">
       <c r="A46" s="20"/>
       <c r="B46" s="20" t="s">
         <v>24</v>
@@ -7493,7 +7512,7 @@
       </c>
       <c r="I46" s="20"/>
     </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15">
       <c r="A47" s="20"/>
       <c r="B47" s="20" t="s">
         <v>24</v>
@@ -7516,7 +7535,7 @@
       </c>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15">
       <c r="A48" s="20"/>
       <c r="B48" s="20" t="s">
         <v>24</v>
@@ -7539,7 +7558,7 @@
       </c>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15">
       <c r="A49" s="20"/>
       <c r="B49" s="20" t="s">
         <v>24</v>
@@ -7562,7 +7581,7 @@
       </c>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15">
       <c r="A50" s="20"/>
       <c r="B50" s="20" t="s">
         <v>24</v>
@@ -7585,7 +7604,7 @@
       </c>
       <c r="I50" s="20"/>
     </row>
-    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15">
       <c r="A51" s="20" t="b">
         <v>0</v>
       </c>
@@ -7604,7 +7623,7 @@
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15">
       <c r="A52" s="20"/>
       <c r="B52" s="20" t="s">
         <v>24</v>
@@ -7625,7 +7644,7 @@
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15">
       <c r="A53" s="20"/>
       <c r="B53" s="20" t="s">
         <v>24</v>
@@ -7648,7 +7667,7 @@
       </c>
       <c r="I53" s="20"/>
     </row>
-    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15">
       <c r="A54" s="20"/>
       <c r="B54" s="20" t="s">
         <v>24</v>
@@ -7671,7 +7690,7 @@
       </c>
       <c r="I54" s="20"/>
     </row>
-    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15">
       <c r="A55" s="20"/>
       <c r="B55" s="20" t="s">
         <v>24</v>
@@ -7694,7 +7713,7 @@
       </c>
       <c r="I55" s="20"/>
     </row>
-    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15">
       <c r="A56" s="20"/>
       <c r="B56" s="20" t="s">
         <v>24</v>
@@ -7717,7 +7736,7 @@
       </c>
       <c r="I56" s="20"/>
     </row>
-    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15">
       <c r="A57" s="20"/>
       <c r="B57" s="20" t="s">
         <v>24</v>
@@ -7740,7 +7759,7 @@
       </c>
       <c r="I57" s="20"/>
     </row>
-    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15">
       <c r="A58" s="20"/>
       <c r="B58" s="20" t="s">
         <v>24</v>
@@ -7763,7 +7782,7 @@
       </c>
       <c r="I58" s="20"/>
     </row>
-    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15">
       <c r="A59" s="20"/>
       <c r="B59" s="20" t="s">
         <v>24</v>
@@ -7786,7 +7805,7 @@
       </c>
       <c r="I59" s="20"/>
     </row>
-    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15">
       <c r="A60" s="20"/>
       <c r="B60" s="20" t="s">
         <v>24</v>
@@ -7809,7 +7828,7 @@
       </c>
       <c r="I60" s="20"/>
     </row>
-    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15">
       <c r="A61" s="20" t="b">
         <v>0</v>
       </c>
@@ -7828,7 +7847,7 @@
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
     </row>
-    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="15">
       <c r="A62" s="20"/>
       <c r="B62" s="20" t="s">
         <v>24</v>
@@ -7849,7 +7868,7 @@
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
     </row>
-    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15">
       <c r="A63" s="20"/>
       <c r="B63" s="20" t="s">
         <v>24</v>
@@ -7874,7 +7893,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15">
       <c r="A64" s="20"/>
       <c r="B64" s="20" t="s">
         <v>24</v>
@@ -7897,7 +7916,7 @@
       </c>
       <c r="I64" s="20"/>
     </row>
-    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="15">
       <c r="A65" s="20"/>
       <c r="B65" s="20" t="s">
         <v>24</v>
@@ -7920,7 +7939,7 @@
       </c>
       <c r="I65" s="20"/>
     </row>
-    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="15">
       <c r="A66" s="20"/>
       <c r="B66" s="20" t="s">
         <v>24</v>
@@ -7943,7 +7962,7 @@
       </c>
       <c r="I66" s="20"/>
     </row>
-    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="15">
       <c r="A67" s="20"/>
       <c r="B67" s="20" t="s">
         <v>24</v>
@@ -7966,7 +7985,7 @@
       </c>
       <c r="I67" s="20"/>
     </row>
-    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="15">
       <c r="A68" s="20"/>
       <c r="B68" s="20" t="s">
         <v>24</v>
@@ -7989,7 +8008,7 @@
       </c>
       <c r="I68" s="20"/>
     </row>
-    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="15">
       <c r="A69" s="20"/>
       <c r="B69" s="20" t="s">
         <v>24</v>
@@ -8012,7 +8031,7 @@
       </c>
       <c r="I69" s="20"/>
     </row>
-    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="15">
       <c r="A70" s="20"/>
       <c r="B70" s="20" t="s">
         <v>24</v>
@@ -8035,7 +8054,7 @@
       </c>
       <c r="I70" s="20"/>
     </row>
-    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="15">
       <c r="A71" s="20"/>
       <c r="B71" s="20" t="s">
         <v>24</v>
@@ -8058,7 +8077,7 @@
       </c>
       <c r="I71" s="20"/>
     </row>
-    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="15">
       <c r="A72" s="20" t="b">
         <v>0</v>
       </c>
@@ -8077,7 +8096,7 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
     </row>
-    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="15">
       <c r="A73" s="20"/>
       <c r="B73" s="20" t="s">
         <v>24</v>
@@ -8098,7 +8117,7 @@
       <c r="H73" s="20"/>
       <c r="I73" s="20"/>
     </row>
-    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="15">
       <c r="A74" s="20"/>
       <c r="B74" s="20" t="s">
         <v>24</v>
@@ -8121,7 +8140,7 @@
       </c>
       <c r="I74" s="20"/>
     </row>
-    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="15">
       <c r="A75" s="20"/>
       <c r="B75" s="20" t="s">
         <v>24</v>
@@ -8146,7 +8165,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="15">
       <c r="A76" s="20"/>
       <c r="B76" s="20" t="s">
         <v>24</v>
@@ -8169,7 +8188,7 @@
       </c>
       <c r="I76" s="20"/>
     </row>
-    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="15">
       <c r="A77" s="20"/>
       <c r="B77" s="20" t="s">
         <v>24</v>
@@ -8192,7 +8211,7 @@
       </c>
       <c r="I77" s="20"/>
     </row>
-    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="15">
       <c r="A78" s="20"/>
       <c r="B78" s="20" t="s">
         <v>24</v>
@@ -8215,7 +8234,7 @@
       </c>
       <c r="I78" s="20"/>
     </row>
-    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="15">
       <c r="A79" s="20"/>
       <c r="B79" s="20" t="s">
         <v>24</v>
@@ -8238,7 +8257,7 @@
       </c>
       <c r="I79" s="20"/>
     </row>
-    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="15">
       <c r="A80" s="20"/>
       <c r="B80" s="20" t="s">
         <v>24</v>
@@ -8261,7 +8280,7 @@
       </c>
       <c r="I80" s="20"/>
     </row>
-    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="15">
       <c r="A81" s="20"/>
       <c r="B81" s="20" t="s">
         <v>24</v>
@@ -8284,7 +8303,7 @@
       </c>
       <c r="I81" s="20"/>
     </row>
-    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="15">
       <c r="A82" s="20"/>
       <c r="B82" s="20" t="s">
         <v>24</v>
@@ -8307,7 +8326,7 @@
       </c>
       <c r="I82" s="20"/>
     </row>
-    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="15">
       <c r="A83" s="20"/>
       <c r="B83" s="20" t="s">
         <v>24</v>
@@ -8330,7 +8349,7 @@
       </c>
       <c r="I83" s="20"/>
     </row>
-    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="15">
       <c r="A84" s="20"/>
       <c r="B84" s="20" t="s">
         <v>24</v>
@@ -8353,7 +8372,7 @@
       </c>
       <c r="I84" s="20"/>
     </row>
-    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="15">
       <c r="A85" s="20"/>
       <c r="B85" s="20" t="s">
         <v>24</v>
@@ -8376,7 +8395,7 @@
       </c>
       <c r="I85" s="20"/>
     </row>
-    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="15">
       <c r="A86" s="20" t="b">
         <v>0</v>
       </c>
@@ -8395,7 +8414,7 @@
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
     </row>
-    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="15">
       <c r="A87" s="20"/>
       <c r="B87" s="20" t="s">
         <v>24</v>
@@ -8418,7 +8437,7 @@
       </c>
       <c r="I87" s="20"/>
     </row>
-    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="15">
       <c r="A88" s="20"/>
       <c r="B88" s="20" t="s">
         <v>24</v>
@@ -8441,7 +8460,7 @@
       </c>
       <c r="I88" s="20"/>
     </row>
-    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="15">
       <c r="A89" s="20"/>
       <c r="B89" s="20" t="s">
         <v>24</v>
@@ -8464,7 +8483,7 @@
       </c>
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="15">
       <c r="A90" s="20"/>
       <c r="B90" s="20" t="s">
         <v>24</v>
@@ -8487,7 +8506,7 @@
       </c>
       <c r="I90" s="20"/>
     </row>
-    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="15">
       <c r="A91" s="20"/>
       <c r="B91" s="20" t="s">
         <v>24</v>
@@ -8510,7 +8529,7 @@
       </c>
       <c r="I91" s="20"/>
     </row>
-    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="15">
       <c r="A92" s="20"/>
       <c r="B92" s="20" t="s">
         <v>24</v>
@@ -8533,7 +8552,7 @@
       </c>
       <c r="I92" s="20"/>
     </row>
-    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="15">
       <c r="A93" s="20"/>
       <c r="B93" s="20" t="s">
         <v>24</v>
@@ -8556,7 +8575,7 @@
       </c>
       <c r="I93" s="20"/>
     </row>
-    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="15">
       <c r="A94" s="20"/>
       <c r="B94" s="20" t="s">
         <v>24</v>
@@ -8579,7 +8598,7 @@
       </c>
       <c r="I94" s="20"/>
     </row>
-    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="15">
       <c r="A95" s="20"/>
       <c r="B95" s="20" t="s">
         <v>24</v>
@@ -8602,7 +8621,7 @@
       </c>
       <c r="I95" s="20"/>
     </row>
-    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="15">
       <c r="A96" s="20"/>
       <c r="B96" s="20" t="s">
         <v>24</v>
@@ -8625,7 +8644,7 @@
       </c>
       <c r="I96" s="20"/>
     </row>
-    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="15">
       <c r="A97" s="20" t="b">
         <v>0</v>
       </c>
@@ -8644,7 +8663,7 @@
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
     </row>
-    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="15">
       <c r="A98" s="20"/>
       <c r="B98" s="20" t="s">
         <v>24</v>
@@ -8669,7 +8688,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="15">
       <c r="A99" s="20" t="b">
         <v>0</v>
       </c>
@@ -8688,7 +8707,7 @@
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
     </row>
-    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="15">
       <c r="A100" s="20"/>
       <c r="B100" s="20" t="s">
         <v>24</v>
@@ -8709,7 +8728,7 @@
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
     </row>
-    <row r="101" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="19" customHeight="1">
       <c r="A101" s="20"/>
       <c r="B101" s="20" t="s">
         <v>24</v>
@@ -8734,7 +8753,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="15">
       <c r="A102" s="20" t="b">
         <v>0</v>
       </c>
@@ -8753,7 +8772,7 @@
       <c r="H102" s="20"/>
       <c r="I102" s="20"/>
     </row>
-    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="15">
       <c r="A103" s="20"/>
       <c r="B103" s="20" t="s">
         <v>24</v>
@@ -8776,7 +8795,7 @@
       </c>
       <c r="I103" s="20"/>
     </row>
-    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="15">
       <c r="A104" s="20"/>
       <c r="B104" s="20" t="s">
         <v>24</v>
@@ -8801,7 +8820,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="15">
       <c r="A105" s="20"/>
       <c r="B105" s="20" t="s">
         <v>24</v>
@@ -8824,7 +8843,7 @@
       </c>
       <c r="I105" s="20"/>
     </row>
-    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="15">
       <c r="A106" s="20"/>
       <c r="B106" s="20" t="s">
         <v>24</v>
@@ -8845,7 +8864,7 @@
       <c r="H106" s="20"/>
       <c r="I106" s="20"/>
     </row>
-    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="15">
       <c r="A107" s="20" t="b">
         <v>0</v>
       </c>
@@ -8864,7 +8883,7 @@
       <c r="H107" s="20"/>
       <c r="I107" s="20"/>
     </row>
-    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="15">
       <c r="A108" s="20"/>
       <c r="B108" s="20" t="s">
         <v>24</v>
@@ -8889,7 +8908,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="15">
       <c r="A109" s="20"/>
       <c r="B109" s="20" t="s">
         <v>24</v>
@@ -8912,7 +8931,7 @@
       </c>
       <c r="I109" s="20"/>
     </row>
-    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="15">
       <c r="A110" s="20"/>
       <c r="B110" s="20" t="s">
         <v>24</v>
@@ -8935,7 +8954,7 @@
       </c>
       <c r="I110" s="20"/>
     </row>
-    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="15">
       <c r="A111" s="20"/>
       <c r="B111" s="20" t="s">
         <v>24</v>
@@ -8958,7 +8977,7 @@
       </c>
       <c r="I111" s="20"/>
     </row>
-    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="15">
       <c r="A112" s="20"/>
       <c r="B112" s="20" t="s">
         <v>24</v>
@@ -8981,7 +9000,7 @@
       </c>
       <c r="I112" s="20"/>
     </row>
-    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="15">
       <c r="A113" s="20"/>
       <c r="B113" s="20" t="s">
         <v>24</v>
@@ -9004,7 +9023,7 @@
       </c>
       <c r="I113" s="20"/>
     </row>
-    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="15">
       <c r="A114" s="20"/>
       <c r="B114" s="20" t="s">
         <v>24</v>
@@ -9027,7 +9046,7 @@
       </c>
       <c r="I114" s="20"/>
     </row>
-    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="15">
       <c r="A115" s="20" t="b">
         <v>0</v>
       </c>
@@ -9046,7 +9065,7 @@
       <c r="H115" s="20"/>
       <c r="I115" s="20"/>
     </row>
-    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="15">
       <c r="A116" s="20"/>
       <c r="B116" s="20" t="s">
         <v>24</v>
@@ -9069,7 +9088,7 @@
       </c>
       <c r="I116" s="20"/>
     </row>
-    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="15">
       <c r="A117" s="20"/>
       <c r="B117" s="20" t="s">
         <v>24</v>
@@ -9092,7 +9111,7 @@
       </c>
       <c r="I117" s="20"/>
     </row>
-    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="15">
       <c r="A118" s="20"/>
       <c r="B118" s="20" t="s">
         <v>24</v>
@@ -9115,7 +9134,7 @@
       </c>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="15">
       <c r="A119" s="20" t="b">
         <v>0</v>
       </c>
@@ -9134,7 +9153,7 @@
       <c r="H119" s="20"/>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="15">
       <c r="A120" s="20"/>
       <c r="B120" s="20" t="s">
         <v>24</v>
@@ -9157,7 +9176,7 @@
       </c>
       <c r="I120" s="20"/>
     </row>
-    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="15">
       <c r="A121" s="20"/>
       <c r="B121" s="20" t="s">
         <v>24</v>
@@ -9180,7 +9199,7 @@
       </c>
       <c r="I121" s="20"/>
     </row>
-    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="15">
       <c r="A122" s="20"/>
       <c r="B122" s="20" t="s">
         <v>24</v>
@@ -9203,7 +9222,7 @@
       </c>
       <c r="I122" s="20"/>
     </row>
-    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="15">
       <c r="A123" s="20"/>
       <c r="B123" s="20" t="s">
         <v>24</v>
@@ -9226,7 +9245,7 @@
       </c>
       <c r="I123" s="20"/>
     </row>
-    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="15">
       <c r="A124" s="20"/>
       <c r="B124" s="20" t="s">
         <v>24</v>
@@ -9249,7 +9268,7 @@
       </c>
       <c r="I124" s="20"/>
     </row>
-    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="15">
       <c r="A125" s="20"/>
       <c r="B125" s="20" t="s">
         <v>24</v>
@@ -9272,7 +9291,7 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="15">
       <c r="A126" s="20" t="b">
         <v>0</v>
       </c>
@@ -9291,7 +9310,7 @@
       <c r="H126" s="20"/>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="15">
       <c r="A127" s="20"/>
       <c r="B127" s="20" t="s">
         <v>24</v>
@@ -9316,7 +9335,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="15">
       <c r="A128" s="20"/>
       <c r="B128" s="20" t="s">
         <v>24</v>
@@ -9339,7 +9358,7 @@
       </c>
       <c r="I128" s="20"/>
     </row>
-    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="15">
       <c r="A129" s="20"/>
       <c r="B129" s="20" t="s">
         <v>24</v>
@@ -9362,7 +9381,7 @@
       </c>
       <c r="I129" s="20"/>
     </row>
-    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="15">
       <c r="A130" s="20"/>
       <c r="B130" s="20" t="s">
         <v>24</v>
@@ -9385,7 +9404,7 @@
       </c>
       <c r="I130" s="20"/>
     </row>
-    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" ht="15">
       <c r="A131" s="20"/>
       <c r="B131" s="20" t="s">
         <v>24</v>
@@ -9408,7 +9427,7 @@
       </c>
       <c r="I131" s="20"/>
     </row>
-    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="15">
       <c r="A132" s="20"/>
       <c r="B132" s="20" t="s">
         <v>24</v>
@@ -9431,7 +9450,7 @@
       </c>
       <c r="I132" s="20"/>
     </row>
-    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" ht="15">
       <c r="A133" s="20"/>
       <c r="B133" s="20" t="s">
         <v>24</v>
@@ -9454,7 +9473,7 @@
       </c>
       <c r="I133" s="20"/>
     </row>
-    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" ht="15">
       <c r="A134" s="20"/>
       <c r="B134" s="20" t="s">
         <v>24</v>
@@ -9477,7 +9496,7 @@
       </c>
       <c r="I134" s="20"/>
     </row>
-    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" ht="15">
       <c r="A135" s="20"/>
       <c r="B135" s="20" t="s">
         <v>24</v>
@@ -9500,7 +9519,7 @@
       </c>
       <c r="I135" s="20"/>
     </row>
-    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="15">
       <c r="A136" s="20" t="b">
         <v>0</v>
       </c>
@@ -9519,7 +9538,7 @@
       <c r="H136" s="20"/>
       <c r="I136" s="20"/>
     </row>
-    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="15">
       <c r="A137" s="20"/>
       <c r="B137" s="20" t="s">
         <v>24</v>
@@ -9544,7 +9563,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="15">
       <c r="A138" s="20"/>
       <c r="B138" s="20" t="s">
         <v>24</v>
@@ -9565,7 +9584,7 @@
       <c r="H138" s="20"/>
       <c r="I138" s="20"/>
     </row>
-    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="15">
       <c r="A139" s="20"/>
       <c r="B139" s="20" t="s">
         <v>24</v>
@@ -9588,7 +9607,7 @@
       </c>
       <c r="I139" s="20"/>
     </row>
-    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="15">
       <c r="A140" s="20"/>
       <c r="B140" s="20" t="s">
         <v>24</v>
@@ -9611,7 +9630,7 @@
       </c>
       <c r="I140" s="20"/>
     </row>
-    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="15">
       <c r="A141" s="20"/>
       <c r="B141" s="20" t="s">
         <v>24</v>
@@ -9634,7 +9653,7 @@
       </c>
       <c r="I141" s="20"/>
     </row>
-    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="15">
       <c r="A142" s="20"/>
       <c r="B142" s="20" t="s">
         <v>24</v>
@@ -9657,7 +9676,7 @@
       </c>
       <c r="I142" s="20"/>
     </row>
-    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="15">
       <c r="A143" s="20"/>
       <c r="B143" s="20" t="s">
         <v>24</v>
@@ -9680,7 +9699,7 @@
       </c>
       <c r="I143" s="20"/>
     </row>
-    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="15">
       <c r="A144" s="20"/>
       <c r="B144" s="20" t="s">
         <v>24</v>
@@ -9703,7 +9722,7 @@
       </c>
       <c r="I144" s="20"/>
     </row>
-    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="15">
       <c r="A145" s="20"/>
       <c r="B145" s="20" t="s">
         <v>24</v>
@@ -9726,7 +9745,7 @@
       </c>
       <c r="I145" s="20"/>
     </row>
-    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="15">
       <c r="A146" s="20"/>
       <c r="B146" s="20" t="s">
         <v>24</v>
@@ -9749,7 +9768,7 @@
       </c>
       <c r="I146" s="20"/>
     </row>
-    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" ht="15">
       <c r="A147" s="20"/>
       <c r="B147" s="20" t="s">
         <v>24</v>
@@ -9772,7 +9791,7 @@
       </c>
       <c r="I147" s="20"/>
     </row>
-    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" ht="15">
       <c r="A148" s="20"/>
       <c r="B148" s="20" t="s">
         <v>24</v>
@@ -9795,7 +9814,7 @@
       </c>
       <c r="I148" s="20"/>
     </row>
-    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="15">
       <c r="A149" s="20"/>
       <c r="B149" s="20" t="s">
         <v>24</v>
@@ -9818,7 +9837,7 @@
       </c>
       <c r="I149" s="20"/>
     </row>
-    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" ht="15">
       <c r="A150" s="20"/>
       <c r="B150" s="20" t="s">
         <v>24</v>
@@ -9841,7 +9860,7 @@
       </c>
       <c r="I150" s="20"/>
     </row>
-    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" ht="15">
       <c r="A151" s="20" t="b">
         <v>0</v>
       </c>
@@ -9860,7 +9879,7 @@
       <c r="H151" s="20"/>
       <c r="I151" s="20"/>
     </row>
-    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" ht="15">
       <c r="A152" s="20"/>
       <c r="B152" s="20" t="s">
         <v>24</v>
@@ -9883,7 +9902,7 @@
       </c>
       <c r="I152" s="20"/>
     </row>
-    <row r="153" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" ht="15">
       <c r="A153" s="20" t="b">
         <v>0</v>
       </c>
@@ -9902,7 +9921,7 @@
       <c r="H153" s="20"/>
       <c r="I153" s="20"/>
     </row>
-    <row r="154" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" ht="15">
       <c r="A154" s="20"/>
       <c r="B154" s="20" t="s">
         <v>24</v>
@@ -9925,7 +9944,7 @@
       </c>
       <c r="I154" s="20"/>
     </row>
-    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" ht="15">
       <c r="A155" s="20"/>
       <c r="B155" s="20" t="s">
         <v>24</v>
@@ -9948,7 +9967,7 @@
       </c>
       <c r="I155" s="20"/>
     </row>
-    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" ht="15">
       <c r="A156" s="20" t="b">
         <v>0</v>
       </c>
@@ -9967,7 +9986,7 @@
       <c r="H156" s="20"/>
       <c r="I156" s="20"/>
     </row>
-    <row r="157" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" ht="15">
       <c r="A157" s="20"/>
       <c r="B157" s="20" t="s">
         <v>24</v>
@@ -9992,7 +10011,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" ht="15">
       <c r="A158" s="20"/>
       <c r="B158" s="20" t="s">
         <v>24</v>
@@ -10015,7 +10034,7 @@
       </c>
       <c r="I158" s="20"/>
     </row>
-    <row r="159" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" ht="15">
       <c r="A159" s="20"/>
       <c r="B159" s="20" t="s">
         <v>24</v>
@@ -10038,7 +10057,7 @@
       </c>
       <c r="I159" s="20"/>
     </row>
-    <row r="160" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" ht="15">
       <c r="A160" s="20"/>
       <c r="B160" s="20" t="s">
         <v>24</v>
@@ -10061,7 +10080,7 @@
       </c>
       <c r="I160" s="20"/>
     </row>
-    <row r="161" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" ht="15">
       <c r="A161" s="20"/>
       <c r="B161" s="20" t="s">
         <v>24</v>
@@ -10084,7 +10103,7 @@
       </c>
       <c r="I161" s="20"/>
     </row>
-    <row r="162" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" ht="15">
       <c r="A162" s="20"/>
       <c r="B162" s="20" t="s">
         <v>24</v>
@@ -10107,7 +10126,7 @@
       </c>
       <c r="I162" s="20"/>
     </row>
-    <row r="163" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" ht="15">
       <c r="A163" s="20"/>
       <c r="B163" s="20" t="s">
         <v>24</v>
@@ -10130,7 +10149,7 @@
       </c>
       <c r="I163" s="20"/>
     </row>
-    <row r="164" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" ht="15">
       <c r="A164" s="20"/>
       <c r="B164" s="20" t="s">
         <v>24</v>
@@ -10153,7 +10172,7 @@
       </c>
       <c r="I164" s="20"/>
     </row>
-    <row r="165" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" ht="15">
       <c r="A165" s="20"/>
       <c r="B165" s="20" t="s">
         <v>24</v>
@@ -10176,7 +10195,7 @@
       </c>
       <c r="I165" s="20"/>
     </row>
-    <row r="166" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" ht="15">
       <c r="A166" s="20"/>
       <c r="B166" s="20" t="s">
         <v>24</v>
@@ -10199,7 +10218,7 @@
       </c>
       <c r="I166" s="20"/>
     </row>
-    <row r="167" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" ht="15">
       <c r="A167" s="20" t="b">
         <v>0</v>
       </c>
@@ -10218,7 +10237,7 @@
       <c r="H167" s="20"/>
       <c r="I167" s="20"/>
     </row>
-    <row r="168" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" ht="15">
       <c r="A168" s="20"/>
       <c r="B168" s="20" t="s">
         <v>24</v>
@@ -10243,7 +10262,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" ht="15">
       <c r="A169" s="20"/>
       <c r="B169" s="20" t="s">
         <v>24</v>
@@ -10266,7 +10285,7 @@
       </c>
       <c r="I169" s="20"/>
     </row>
-    <row r="170" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" ht="15">
       <c r="A170" s="20"/>
       <c r="B170" s="20" t="s">
         <v>24</v>
@@ -10289,7 +10308,7 @@
       </c>
       <c r="I170" s="20"/>
     </row>
-    <row r="171" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" ht="15">
       <c r="A171" s="20"/>
       <c r="B171" s="20" t="s">
         <v>24</v>
@@ -10312,7 +10331,7 @@
       </c>
       <c r="I171" s="20"/>
     </row>
-    <row r="172" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" ht="15">
       <c r="A172" s="20"/>
       <c r="B172" s="20" t="s">
         <v>24</v>
@@ -10335,7 +10354,7 @@
       </c>
       <c r="I172" s="20"/>
     </row>
-    <row r="173" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" ht="15">
       <c r="A173" s="20"/>
       <c r="B173" s="20" t="s">
         <v>24</v>
@@ -10358,7 +10377,7 @@
       </c>
       <c r="I173" s="20"/>
     </row>
-    <row r="174" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" ht="15">
       <c r="A174" s="20"/>
       <c r="B174" s="20" t="s">
         <v>24</v>
@@ -10381,7 +10400,7 @@
       </c>
       <c r="I174" s="20"/>
     </row>
-    <row r="175" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" ht="15">
       <c r="A175" s="20"/>
       <c r="B175" s="20" t="s">
         <v>24</v>
@@ -10404,7 +10423,7 @@
       </c>
       <c r="I175" s="20"/>
     </row>
-    <row r="176" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" ht="15">
       <c r="A176" s="20"/>
       <c r="B176" s="20" t="s">
         <v>24</v>
@@ -10427,7 +10446,7 @@
       </c>
       <c r="I176" s="20"/>
     </row>
-    <row r="177" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" ht="15">
       <c r="A177" s="20"/>
       <c r="B177" s="20" t="s">
         <v>24</v>
@@ -10450,7 +10469,7 @@
       </c>
       <c r="I177" s="20"/>
     </row>
-    <row r="178" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" ht="15">
       <c r="A178" s="20" t="b">
         <v>0</v>
       </c>
@@ -10469,7 +10488,7 @@
       <c r="H178" s="20"/>
       <c r="I178" s="20"/>
     </row>
-    <row r="179" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" ht="15">
       <c r="A179" s="20"/>
       <c r="B179" s="20" t="s">
         <v>24</v>
@@ -10492,7 +10511,7 @@
       </c>
       <c r="I179" s="20"/>
     </row>
-    <row r="180" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" ht="15">
       <c r="A180" s="20"/>
       <c r="B180" s="20" t="s">
         <v>24</v>
@@ -10515,7 +10534,7 @@
       </c>
       <c r="I180" s="20"/>
     </row>
-    <row r="181" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" ht="15">
       <c r="A181" s="20"/>
       <c r="B181" s="20" t="s">
         <v>24</v>
@@ -10538,7 +10557,7 @@
       </c>
       <c r="I181" s="20"/>
     </row>
-    <row r="182" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" ht="15">
       <c r="A182" s="20"/>
       <c r="B182" s="20" t="s">
         <v>24</v>
@@ -10561,7 +10580,7 @@
       </c>
       <c r="I182" s="20"/>
     </row>
-    <row r="183" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" ht="15">
       <c r="A183" s="20" t="b">
         <v>0</v>
       </c>
@@ -10580,7 +10599,7 @@
       <c r="H183" s="20"/>
       <c r="I183" s="20"/>
     </row>
-    <row r="184" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" ht="15">
       <c r="A184" s="20"/>
       <c r="B184" s="20" t="s">
         <v>24</v>
@@ -10603,7 +10622,7 @@
       </c>
       <c r="I184" s="20"/>
     </row>
-    <row r="185" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" ht="15">
       <c r="A185" s="20"/>
       <c r="B185" s="20" t="s">
         <v>24</v>
@@ -10626,7 +10645,7 @@
       </c>
       <c r="I185" s="20"/>
     </row>
-    <row r="186" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" ht="15">
       <c r="A186" s="20"/>
       <c r="B186" s="20" t="s">
         <v>24</v>
@@ -10649,7 +10668,7 @@
       </c>
       <c r="I186" s="20"/>
     </row>
-    <row r="187" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" ht="15">
       <c r="A187" s="20"/>
       <c r="B187" s="20" t="s">
         <v>24</v>
@@ -10672,7 +10691,7 @@
       </c>
       <c r="I187" s="20"/>
     </row>
-    <row r="188" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="15">
       <c r="A188" s="20" t="b">
         <v>0</v>
       </c>
@@ -10691,7 +10710,7 @@
       <c r="H188" s="20"/>
       <c r="I188" s="20"/>
     </row>
-    <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" ht="15">
       <c r="A189" s="20"/>
       <c r="B189" s="20" t="s">
         <v>24</v>
@@ -10712,7 +10731,7 @@
       <c r="H189" s="20"/>
       <c r="I189" s="20"/>
     </row>
-    <row r="190" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" ht="15">
       <c r="A190" s="20"/>
       <c r="B190" s="20" t="s">
         <v>24</v>
@@ -10735,7 +10754,7 @@
       </c>
       <c r="I190" s="20"/>
     </row>
-    <row r="191" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" ht="15">
       <c r="A191" s="20" t="b">
         <v>0</v>
       </c>
@@ -10754,7 +10773,7 @@
       <c r="H191" s="20"/>
       <c r="I191" s="20"/>
     </row>
-    <row r="192" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" ht="15">
       <c r="A192" s="20"/>
       <c r="B192" s="20" t="s">
         <v>24</v>
@@ -10777,7 +10796,7 @@
       </c>
       <c r="I192" s="20"/>
     </row>
-    <row r="193" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" ht="15">
       <c r="A193" s="20"/>
       <c r="B193" s="20" t="s">
         <v>24</v>
@@ -10802,7 +10821,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" ht="15">
       <c r="A194" s="20"/>
       <c r="B194" s="20" t="s">
         <v>24</v>
@@ -10823,7 +10842,7 @@
       <c r="H194" s="20"/>
       <c r="I194" s="20"/>
     </row>
-    <row r="195" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" ht="15">
       <c r="A195" s="20"/>
       <c r="B195" s="20" t="s">
         <v>24</v>
@@ -10848,7 +10867,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" ht="15">
       <c r="A196" s="20"/>
       <c r="B196" s="20" t="s">
         <v>24</v>
@@ -10873,7 +10892,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" ht="15">
       <c r="A197" s="20" t="b">
         <v>0</v>
       </c>
@@ -10892,7 +10911,7 @@
       <c r="H197" s="20"/>
       <c r="I197" s="20"/>
     </row>
-    <row r="198" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" ht="15">
       <c r="A198" s="20"/>
       <c r="B198" s="20" t="s">
         <v>24</v>
@@ -10917,7 +10936,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" ht="15">
       <c r="A199" s="20"/>
       <c r="B199" s="20" t="s">
         <v>24</v>
@@ -10940,7 +10959,7 @@
       </c>
       <c r="I199" s="20"/>
     </row>
-    <row r="200" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" ht="15">
       <c r="A200" s="20"/>
       <c r="B200" s="20" t="s">
         <v>24</v>
@@ -10963,7 +10982,7 @@
       </c>
       <c r="I200" s="20"/>
     </row>
-    <row r="201" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" ht="15">
       <c r="A201" s="20"/>
       <c r="B201" s="20" t="s">
         <v>24</v>
@@ -10986,7 +11005,7 @@
       </c>
       <c r="I201" s="20"/>
     </row>
-    <row r="202" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" ht="15">
       <c r="A202" s="20"/>
       <c r="B202" s="20" t="s">
         <v>24</v>
@@ -11009,7 +11028,7 @@
       </c>
       <c r="I202" s="20"/>
     </row>
-    <row r="203" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" ht="15">
       <c r="A203" s="20"/>
       <c r="B203" s="20" t="s">
         <v>24</v>
@@ -11032,7 +11051,7 @@
       </c>
       <c r="I203" s="20"/>
     </row>
-    <row r="204" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" ht="15">
       <c r="A204" s="20"/>
       <c r="B204" s="20" t="s">
         <v>24</v>
@@ -11055,7 +11074,7 @@
       </c>
       <c r="I204" s="20"/>
     </row>
-    <row r="205" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" ht="15">
       <c r="A205" s="20"/>
       <c r="B205" s="20" t="s">
         <v>24</v>
@@ -11078,7 +11097,7 @@
       </c>
       <c r="I205" s="20"/>
     </row>
-    <row r="206" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" ht="15">
       <c r="A206" s="20"/>
       <c r="B206" s="20" t="s">
         <v>24</v>
@@ -11101,7 +11120,7 @@
       </c>
       <c r="I206" s="20"/>
     </row>
-    <row r="207" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" ht="15">
       <c r="A207" s="20" t="b">
         <v>0</v>
       </c>
@@ -11120,7 +11139,7 @@
       <c r="H207" s="20"/>
       <c r="I207" s="20"/>
     </row>
-    <row r="208" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" ht="15">
       <c r="A208" s="20"/>
       <c r="B208" s="20" t="s">
         <v>24</v>
@@ -11145,7 +11164,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" ht="15">
       <c r="A209" s="20"/>
       <c r="B209" s="20" t="s">
         <v>24</v>
@@ -11168,7 +11187,7 @@
       </c>
       <c r="I209" s="20"/>
     </row>
-    <row r="210" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" ht="15">
       <c r="A210" s="20"/>
       <c r="B210" s="20" t="s">
         <v>24</v>
@@ -11191,7 +11210,7 @@
       </c>
       <c r="I210" s="20"/>
     </row>
-    <row r="211" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" ht="15">
       <c r="A211" s="20"/>
       <c r="B211" s="20" t="s">
         <v>24</v>
@@ -11214,7 +11233,7 @@
       </c>
       <c r="I211" s="20"/>
     </row>
-    <row r="212" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" ht="15">
       <c r="A212" s="20"/>
       <c r="B212" s="20" t="s">
         <v>24</v>
@@ -11237,7 +11256,7 @@
       </c>
       <c r="I212" s="20"/>
     </row>
-    <row r="213" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" ht="15">
       <c r="A213" s="20"/>
       <c r="B213" s="20" t="s">
         <v>24</v>
@@ -11260,7 +11279,7 @@
       </c>
       <c r="I213" s="20"/>
     </row>
-    <row r="214" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" ht="15">
       <c r="A214" s="20"/>
       <c r="B214" s="20" t="s">
         <v>24</v>
@@ -11283,7 +11302,7 @@
       </c>
       <c r="I214" s="20"/>
     </row>
-    <row r="215" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" ht="15">
       <c r="A215" s="20"/>
       <c r="B215" s="20" t="s">
         <v>24</v>
@@ -11306,7 +11325,7 @@
       </c>
       <c r="I215" s="20"/>
     </row>
-    <row r="216" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" ht="15">
       <c r="A216" s="20"/>
       <c r="B216" s="20" t="s">
         <v>24</v>
@@ -11329,7 +11348,7 @@
       </c>
       <c r="I216" s="20"/>
     </row>
-    <row r="217" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" ht="15">
       <c r="A217" s="20" t="b">
         <v>0</v>
       </c>
@@ -11348,7 +11367,7 @@
       <c r="H217" s="20"/>
       <c r="I217" s="20"/>
     </row>
-    <row r="218" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" ht="15">
       <c r="A218" s="20"/>
       <c r="B218" s="20" t="s">
         <v>24</v>
@@ -11369,7 +11388,7 @@
       <c r="H218" s="20"/>
       <c r="I218" s="20"/>
     </row>
-    <row r="219" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" ht="15">
       <c r="A219" s="20"/>
       <c r="B219" s="20" t="s">
         <v>24</v>
@@ -11392,7 +11411,7 @@
       </c>
       <c r="I219" s="20"/>
     </row>
-    <row r="220" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" ht="15">
       <c r="A220" s="20"/>
       <c r="B220" s="20" t="s">
         <v>24</v>
@@ -11415,7 +11434,7 @@
       </c>
       <c r="I220" s="20"/>
     </row>
-    <row r="221" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" ht="15">
       <c r="A221" s="20"/>
       <c r="B221" s="20" t="s">
         <v>24</v>
@@ -11438,7 +11457,7 @@
       </c>
       <c r="I221" s="20"/>
     </row>
-    <row r="222" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" ht="15">
       <c r="A222" s="20"/>
       <c r="B222" s="20" t="s">
         <v>24</v>
@@ -11461,7 +11480,7 @@
       </c>
       <c r="I222" s="20"/>
     </row>
-    <row r="223" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" ht="15">
       <c r="A223" s="20"/>
       <c r="B223" s="20" t="s">
         <v>24</v>
@@ -11484,7 +11503,7 @@
       </c>
       <c r="I223" s="20"/>
     </row>
-    <row r="224" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" ht="15">
       <c r="A224" s="20"/>
       <c r="B224" s="20" t="s">
         <v>24</v>
@@ -11507,7 +11526,7 @@
       </c>
       <c r="I224" s="20"/>
     </row>
-    <row r="225" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" ht="15">
       <c r="A225" s="20"/>
       <c r="B225" s="20" t="s">
         <v>24</v>
@@ -11530,7 +11549,7 @@
       </c>
       <c r="I225" s="20"/>
     </row>
-    <row r="226" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" ht="15">
       <c r="A226" s="20"/>
       <c r="B226" s="20" t="s">
         <v>24</v>
@@ -11553,7 +11572,7 @@
       </c>
       <c r="I226" s="20"/>
     </row>
-    <row r="227" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" ht="15">
       <c r="A227" s="20"/>
       <c r="B227" s="20" t="s">
         <v>24</v>
@@ -11576,7 +11595,7 @@
       </c>
       <c r="I227" s="20"/>
     </row>
-    <row r="228" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" ht="15">
       <c r="A228" s="20"/>
       <c r="B228" s="20" t="s">
         <v>24</v>
@@ -11599,7 +11618,7 @@
       </c>
       <c r="I228" s="20"/>
     </row>
-    <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" ht="15">
       <c r="A229" s="20"/>
       <c r="B229" s="20" t="s">
         <v>24</v>
@@ -11622,7 +11641,7 @@
       </c>
       <c r="I229" s="20"/>
     </row>
-    <row r="230" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" ht="15">
       <c r="A230" s="20"/>
       <c r="B230" s="20" t="s">
         <v>24</v>
@@ -11645,7 +11664,7 @@
       </c>
       <c r="I230" s="20"/>
     </row>
-    <row r="231" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" ht="15">
       <c r="A231" s="20"/>
       <c r="B231" s="20" t="s">
         <v>24</v>
@@ -11668,7 +11687,7 @@
       </c>
       <c r="I231" s="20"/>
     </row>
-    <row r="232" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" ht="15">
       <c r="A232" s="20"/>
       <c r="B232" s="20" t="s">
         <v>24</v>
@@ -11691,7 +11710,7 @@
       </c>
       <c r="I232" s="20"/>
     </row>
-    <row r="233" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" ht="15">
       <c r="A233" s="20"/>
       <c r="B233" s="20" t="s">
         <v>24</v>
@@ -11714,7 +11733,7 @@
       </c>
       <c r="I233" s="20"/>
     </row>
-    <row r="234" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" ht="15">
       <c r="A234" s="20" t="b">
         <v>0</v>
       </c>
@@ -11733,7 +11752,7 @@
       <c r="H234" s="20"/>
       <c r="I234" s="20"/>
     </row>
-    <row r="235" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" ht="15">
       <c r="A235" s="20"/>
       <c r="B235" s="20" t="s">
         <v>24</v>
@@ -11754,7 +11773,7 @@
       <c r="H235" s="20"/>
       <c r="I235" s="20"/>
     </row>
-    <row r="236" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" ht="15">
       <c r="A236" s="20"/>
       <c r="B236" s="20" t="s">
         <v>24</v>
@@ -11777,7 +11796,7 @@
       </c>
       <c r="I236" s="20"/>
     </row>
-    <row r="237" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" ht="15">
       <c r="A237" s="20"/>
       <c r="B237" s="20" t="s">
         <v>24</v>
@@ -11800,7 +11819,7 @@
       </c>
       <c r="I237" s="20"/>
     </row>
-    <row r="238" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" ht="15">
       <c r="A238" s="20"/>
       <c r="B238" s="20" t="s">
         <v>24</v>
@@ -11823,7 +11842,7 @@
       </c>
       <c r="I238" s="20"/>
     </row>
-    <row r="239" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" ht="15">
       <c r="A239" s="20"/>
       <c r="B239" s="20" t="s">
         <v>24</v>
@@ -11846,7 +11865,7 @@
       </c>
       <c r="I239" s="20"/>
     </row>
-    <row r="240" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" ht="15">
       <c r="A240" s="20"/>
       <c r="B240" s="20" t="s">
         <v>24</v>
@@ -11869,7 +11888,7 @@
       </c>
       <c r="I240" s="20"/>
     </row>
-    <row r="241" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" ht="15">
       <c r="A241" s="20"/>
       <c r="B241" s="20" t="s">
         <v>24</v>
@@ -11892,7 +11911,7 @@
       </c>
       <c r="I241" s="20"/>
     </row>
-    <row r="242" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" ht="15">
       <c r="A242" s="20"/>
       <c r="B242" s="20" t="s">
         <v>24</v>
@@ -11915,7 +11934,7 @@
       </c>
       <c r="I242" s="20"/>
     </row>
-    <row r="243" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" ht="15">
       <c r="A243" s="20"/>
       <c r="B243" s="20" t="s">
         <v>24</v>
@@ -11938,7 +11957,7 @@
       </c>
       <c r="I243" s="20"/>
     </row>
-    <row r="244" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" ht="15">
       <c r="A244" s="20"/>
       <c r="B244" s="20" t="s">
         <v>24</v>
@@ -11961,7 +11980,7 @@
       </c>
       <c r="I244" s="20"/>
     </row>
-    <row r="245" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" ht="15">
       <c r="A245" s="20"/>
       <c r="B245" s="20" t="s">
         <v>24</v>
@@ -11984,7 +12003,7 @@
       </c>
       <c r="I245" s="20"/>
     </row>
-    <row r="246" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" ht="15">
       <c r="A246" s="20"/>
       <c r="B246" s="20" t="s">
         <v>24</v>
@@ -12007,7 +12026,7 @@
       </c>
       <c r="I246" s="20"/>
     </row>
-    <row r="247" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" ht="15">
       <c r="A247" s="20"/>
       <c r="B247" s="20" t="s">
         <v>24</v>
@@ -12030,7 +12049,7 @@
       </c>
       <c r="I247" s="20"/>
     </row>
-    <row r="248" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" ht="15">
       <c r="A248" s="20"/>
       <c r="B248" s="20" t="s">
         <v>24</v>
@@ -12053,7 +12072,7 @@
       </c>
       <c r="I248" s="20"/>
     </row>
-    <row r="249" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" ht="15">
       <c r="A249" s="20"/>
       <c r="B249" s="20" t="s">
         <v>24</v>
@@ -12076,7 +12095,7 @@
       </c>
       <c r="I249" s="20"/>
     </row>
-    <row r="250" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" ht="15">
       <c r="A250" s="20"/>
       <c r="B250" s="20" t="s">
         <v>24</v>
@@ -12099,7 +12118,7 @@
       </c>
       <c r="I250" s="20"/>
     </row>
-    <row r="251" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" ht="15">
       <c r="A251" s="20" t="b">
         <v>0</v>
       </c>
@@ -12118,7 +12137,7 @@
       <c r="H251" s="20"/>
       <c r="I251" s="20"/>
     </row>
-    <row r="252" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" ht="15">
       <c r="A252" s="20"/>
       <c r="B252" s="20" t="s">
         <v>24</v>
@@ -12143,7 +12162,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" ht="15">
       <c r="A253" s="20"/>
       <c r="B253" s="20" t="s">
         <v>24</v>
@@ -12166,7 +12185,7 @@
       </c>
       <c r="I253" s="20"/>
     </row>
-    <row r="254" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" ht="15">
       <c r="A254" s="20"/>
       <c r="B254" s="20" t="s">
         <v>24</v>
@@ -12189,7 +12208,7 @@
       </c>
       <c r="I254" s="20"/>
     </row>
-    <row r="255" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" ht="15">
       <c r="A255" s="20"/>
       <c r="B255" s="20" t="s">
         <v>24</v>
@@ -12212,7 +12231,7 @@
       </c>
       <c r="I255" s="20"/>
     </row>
-    <row r="256" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" ht="15">
       <c r="A256" s="20"/>
       <c r="B256" s="20" t="s">
         <v>24</v>
@@ -12235,7 +12254,7 @@
       </c>
       <c r="I256" s="20"/>
     </row>
-    <row r="257" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" ht="15">
       <c r="A257" s="20" t="b">
         <v>0</v>
       </c>
@@ -12254,7 +12273,7 @@
       <c r="H257" s="20"/>
       <c r="I257" s="20"/>
     </row>
-    <row r="258" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" ht="15">
       <c r="A258" s="20"/>
       <c r="B258" s="20" t="s">
         <v>24</v>
@@ -12279,7 +12298,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" ht="15">
       <c r="A259" s="20"/>
       <c r="B259" s="20" t="s">
         <v>24</v>
@@ -12302,7 +12321,7 @@
       </c>
       <c r="I259" s="20"/>
     </row>
-    <row r="260" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" ht="15">
       <c r="A260" s="20" t="b">
         <v>0</v>
       </c>
@@ -12321,7 +12340,7 @@
       <c r="H260" s="20"/>
       <c r="I260" s="20"/>
     </row>
-    <row r="261" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" ht="15">
       <c r="A261" s="20" t="b">
         <v>0</v>
       </c>
@@ -12340,7 +12359,7 @@
       <c r="H261" s="20"/>
       <c r="I261" s="20"/>
     </row>
-    <row r="262" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" ht="15">
       <c r="A262" s="20" t="b">
         <v>0</v>
       </c>
@@ -12359,7 +12378,7 @@
       <c r="H262" s="20"/>
       <c r="I262" s="20"/>
     </row>
-    <row r="263" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" ht="15">
       <c r="A263" s="20"/>
       <c r="B263" s="20" t="s">
         <v>24</v>
@@ -12380,7 +12399,7 @@
       <c r="H263" s="20"/>
       <c r="I263" s="20"/>
     </row>
-    <row r="264" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" ht="15">
       <c r="A264" s="20"/>
       <c r="B264" s="20" t="s">
         <v>24</v>
@@ -12403,7 +12422,7 @@
       </c>
       <c r="I264" s="20"/>
     </row>
-    <row r="265" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" ht="15">
       <c r="A265" s="20"/>
       <c r="B265" s="20" t="s">
         <v>24</v>
@@ -12426,7 +12445,7 @@
       </c>
       <c r="I265" s="20"/>
     </row>
-    <row r="266" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" ht="15">
       <c r="A266" s="20"/>
       <c r="B266" s="20" t="s">
         <v>24</v>
@@ -12449,7 +12468,7 @@
       </c>
       <c r="I266" s="20"/>
     </row>
-    <row r="267" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" ht="15">
       <c r="A267" s="20"/>
       <c r="B267" s="20" t="s">
         <v>24</v>
@@ -12472,7 +12491,7 @@
       </c>
       <c r="I267" s="20"/>
     </row>
-    <row r="268" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" ht="15">
       <c r="A268" s="20"/>
       <c r="B268" s="20" t="s">
         <v>24</v>
@@ -12495,7 +12514,7 @@
       </c>
       <c r="I268" s="20"/>
     </row>
-    <row r="269" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" ht="15">
       <c r="A269" s="20"/>
       <c r="B269" s="20" t="s">
         <v>24</v>
@@ -12518,7 +12537,7 @@
       </c>
       <c r="I269" s="20"/>
     </row>
-    <row r="270" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" ht="15">
       <c r="A270" s="20"/>
       <c r="B270" s="20" t="s">
         <v>24</v>
@@ -12541,7 +12560,7 @@
       </c>
       <c r="I270" s="20"/>
     </row>
-    <row r="271" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" ht="15">
       <c r="A271" s="20"/>
       <c r="B271" s="20" t="s">
         <v>24</v>
@@ -12564,7 +12583,7 @@
       </c>
       <c r="I271" s="20"/>
     </row>
-    <row r="272" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" ht="15">
       <c r="A272" s="20"/>
       <c r="B272" s="20" t="s">
         <v>24</v>
@@ -12587,7 +12606,7 @@
       </c>
       <c r="I272" s="20"/>
     </row>
-    <row r="273" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" ht="15">
       <c r="A273" s="20"/>
       <c r="B273" s="20" t="s">
         <v>24</v>
@@ -12610,7 +12629,7 @@
       </c>
       <c r="I273" s="20"/>
     </row>
-    <row r="274" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" ht="15">
       <c r="A274" s="20" t="b">
         <v>0</v>
       </c>
@@ -12629,7 +12648,7 @@
       <c r="H274" s="20"/>
       <c r="I274" s="20"/>
     </row>
-    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" ht="15">
       <c r="A275" s="20"/>
       <c r="B275" s="20" t="s">
         <v>24</v>
@@ -12652,7 +12671,7 @@
       </c>
       <c r="I275" s="20"/>
     </row>
-    <row r="276" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" ht="15">
       <c r="A276" s="20" t="b">
         <v>0</v>
       </c>
@@ -12671,7 +12690,7 @@
       <c r="H276" s="20"/>
       <c r="I276" s="20"/>
     </row>
-    <row r="277" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" ht="15">
       <c r="A277" s="20"/>
       <c r="B277" s="20" t="s">
         <v>24</v>
@@ -12696,7 +12715,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" ht="15">
       <c r="A278" s="20"/>
       <c r="B278" s="20" t="s">
         <v>24</v>
@@ -12719,7 +12738,7 @@
       </c>
       <c r="I278" s="20"/>
     </row>
-    <row r="279" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" ht="15">
       <c r="A279" s="20"/>
       <c r="B279" s="20" t="s">
         <v>24</v>
@@ -12742,7 +12761,7 @@
       </c>
       <c r="I279" s="20"/>
     </row>
-    <row r="280" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" ht="15">
       <c r="A280" s="20"/>
       <c r="B280" s="20" t="s">
         <v>24</v>
@@ -12765,7 +12784,7 @@
       </c>
       <c r="I280" s="20"/>
     </row>
-    <row r="281" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" ht="15">
       <c r="A281" s="20"/>
       <c r="B281" s="20" t="s">
         <v>24</v>
@@ -12788,7 +12807,7 @@
       </c>
       <c r="I281" s="20"/>
     </row>
-    <row r="282" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" ht="15">
       <c r="A282" s="20"/>
       <c r="B282" s="20" t="s">
         <v>24</v>
@@ -12811,7 +12830,7 @@
       </c>
       <c r="I282" s="20"/>
     </row>
-    <row r="283" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" ht="15">
       <c r="A283" s="20"/>
       <c r="B283" s="20" t="s">
         <v>24</v>
@@ -12834,7 +12853,7 @@
       </c>
       <c r="I283" s="20"/>
     </row>
-    <row r="284" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" ht="15">
       <c r="A284" s="20"/>
       <c r="B284" s="20" t="s">
         <v>24</v>
@@ -12857,7 +12876,7 @@
       </c>
       <c r="I284" s="20"/>
     </row>
-    <row r="285" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" ht="15">
       <c r="A285" s="20"/>
       <c r="B285" s="20" t="s">
         <v>24</v>
@@ -12880,7 +12899,7 @@
       </c>
       <c r="I285" s="20"/>
     </row>
-    <row r="286" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" ht="15">
       <c r="A286" s="20"/>
       <c r="B286" s="20" t="s">
         <v>24</v>
@@ -12903,7 +12922,7 @@
       </c>
       <c r="I286" s="20"/>
     </row>
-    <row r="287" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" ht="15">
       <c r="A287" s="20"/>
       <c r="B287" s="20" t="s">
         <v>24</v>
@@ -12926,7 +12945,7 @@
       </c>
       <c r="I287" s="20"/>
     </row>
-    <row r="288" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" ht="15">
       <c r="A288" s="20" t="b">
         <v>0</v>
       </c>
@@ -12945,7 +12964,7 @@
       <c r="H288" s="20"/>
       <c r="I288" s="20"/>
     </row>
-    <row r="289" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" ht="15">
       <c r="A289" s="20"/>
       <c r="B289" s="20" t="s">
         <v>24</v>
@@ -12968,7 +12987,7 @@
       </c>
       <c r="I289" s="20"/>
     </row>
-    <row r="290" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" ht="15">
       <c r="A290" s="20" t="b">
         <v>0</v>
       </c>
@@ -12987,7 +13006,7 @@
       <c r="H290" s="20"/>
       <c r="I290" s="20"/>
     </row>
-    <row r="291" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" ht="15">
       <c r="A291" s="20"/>
       <c r="B291" s="20" t="s">
         <v>24</v>
@@ -13008,7 +13027,7 @@
       <c r="H291" s="20"/>
       <c r="I291" s="20"/>
     </row>
-    <row r="292" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" ht="15">
       <c r="A292" s="20" t="b">
         <v>0</v>
       </c>
@@ -13027,7 +13046,7 @@
       <c r="H292" s="20"/>
       <c r="I292" s="20"/>
     </row>
-    <row r="293" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" ht="15">
       <c r="A293" s="20"/>
       <c r="B293" s="20" t="s">
         <v>24</v>
@@ -13048,7 +13067,7 @@
       <c r="H293" s="20"/>
       <c r="I293" s="20"/>
     </row>
-    <row r="294" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" ht="15">
       <c r="A294" s="20" t="b">
         <v>0</v>
       </c>
@@ -13067,7 +13086,7 @@
       <c r="H294" s="20"/>
       <c r="I294" s="20"/>
     </row>
-    <row r="295" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" ht="15">
       <c r="A295" s="20"/>
       <c r="B295" s="20" t="s">
         <v>24</v>
@@ -13088,7 +13107,7 @@
       <c r="H295" s="20"/>
       <c r="I295" s="20"/>
     </row>
-    <row r="296" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" ht="15">
       <c r="A296" s="20" t="b">
         <v>0</v>
       </c>
@@ -13107,7 +13126,7 @@
       <c r="H296" s="20"/>
       <c r="I296" s="20"/>
     </row>
-    <row r="297" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" ht="15">
       <c r="A297" s="20"/>
       <c r="B297" s="20" t="s">
         <v>24</v>
@@ -13130,7 +13149,7 @@
       </c>
       <c r="I297" s="20"/>
     </row>
-    <row r="298" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" ht="15">
       <c r="A298" s="20" t="b">
         <v>0</v>
       </c>
@@ -13149,7 +13168,7 @@
       <c r="H298" s="20"/>
       <c r="I298" s="20"/>
     </row>
-    <row r="299" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" ht="15">
       <c r="A299" s="20"/>
       <c r="B299" s="20" t="s">
         <v>24</v>
@@ -13174,7 +13193,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" ht="15">
       <c r="A300" s="20"/>
       <c r="B300" s="20" t="s">
         <v>24</v>
@@ -13197,7 +13216,7 @@
       </c>
       <c r="I300" s="20"/>
     </row>
-    <row r="301" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" ht="15">
       <c r="A301" s="20"/>
       <c r="B301" s="20" t="s">
         <v>24</v>
@@ -13220,7 +13239,7 @@
       </c>
       <c r="I301" s="20"/>
     </row>
-    <row r="302" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" ht="15">
       <c r="A302" s="20"/>
       <c r="B302" s="20" t="s">
         <v>24</v>
@@ -13243,7 +13262,7 @@
       </c>
       <c r="I302" s="20"/>
     </row>
-    <row r="303" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" ht="15">
       <c r="A303" s="20"/>
       <c r="B303" s="20" t="s">
         <v>24</v>
@@ -13266,7 +13285,7 @@
       </c>
       <c r="I303" s="20"/>
     </row>
-    <row r="304" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" ht="15">
       <c r="A304" s="20"/>
       <c r="B304" s="20" t="s">
         <v>24</v>
@@ -13289,7 +13308,7 @@
       </c>
       <c r="I304" s="20"/>
     </row>
-    <row r="305" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" ht="15">
       <c r="A305" s="20"/>
       <c r="B305" s="20" t="s">
         <v>24</v>
@@ -13312,7 +13331,7 @@
       </c>
       <c r="I305" s="20"/>
     </row>
-    <row r="306" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" ht="15">
       <c r="A306" s="20"/>
       <c r="B306" s="20" t="s">
         <v>24</v>
@@ -13335,7 +13354,7 @@
       </c>
       <c r="I306" s="20"/>
     </row>
-    <row r="307" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" ht="15">
       <c r="A307" s="20"/>
       <c r="B307" s="20" t="s">
         <v>24</v>
@@ -13358,7 +13377,7 @@
       </c>
       <c r="I307" s="20"/>
     </row>
-    <row r="308" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" ht="15">
       <c r="A308" s="20" t="b">
         <v>0</v>
       </c>
@@ -13377,7 +13396,7 @@
       <c r="H308" s="20"/>
       <c r="I308" s="20"/>
     </row>
-    <row r="309" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" ht="15">
       <c r="A309" s="20"/>
       <c r="B309" s="20" t="s">
         <v>24</v>
@@ -13400,7 +13419,7 @@
       </c>
       <c r="I309" s="20"/>
     </row>
-    <row r="310" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" ht="15">
       <c r="A310" s="20"/>
       <c r="B310" s="20" t="s">
         <v>24</v>
@@ -13423,7 +13442,7 @@
       </c>
       <c r="I310" s="20"/>
     </row>
-    <row r="311" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" ht="15">
       <c r="A311" s="20"/>
       <c r="B311" s="20" t="s">
         <v>24</v>
@@ -13446,7 +13465,7 @@
       </c>
       <c r="I311" s="20"/>
     </row>
-    <row r="312" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" ht="15">
       <c r="A312" s="20"/>
       <c r="B312" s="20" t="s">
         <v>24</v>
@@ -13469,7 +13488,7 @@
       </c>
       <c r="I312" s="20"/>
     </row>
-    <row r="313" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" ht="15">
       <c r="A313" s="20" t="b">
         <v>0</v>
       </c>
@@ -13488,7 +13507,7 @@
       <c r="H313" s="20"/>
       <c r="I313" s="20"/>
     </row>
-    <row r="314" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" ht="15">
       <c r="A314" s="20"/>
       <c r="B314" s="20" t="s">
         <v>24</v>
@@ -13511,7 +13530,7 @@
       </c>
       <c r="I314" s="20"/>
     </row>
-    <row r="315" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" ht="15">
       <c r="A315" s="20"/>
       <c r="B315" s="20" t="s">
         <v>24</v>
@@ -13534,7 +13553,7 @@
       </c>
       <c r="I315" s="20"/>
     </row>
-    <row r="316" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" ht="15">
       <c r="A316" s="20"/>
       <c r="B316" s="20" t="s">
         <v>24</v>
@@ -13559,7 +13578,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" ht="15">
       <c r="A317" s="20" t="b">
         <v>0</v>
       </c>
@@ -13578,7 +13597,7 @@
       <c r="H317" s="20"/>
       <c r="I317" s="20"/>
     </row>
-    <row r="318" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" ht="15">
       <c r="A318" s="20"/>
       <c r="B318" s="20" t="s">
         <v>24</v>
@@ -13603,7 +13622,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" ht="15">
       <c r="A319" s="20"/>
       <c r="B319" s="20" t="s">
         <v>24</v>
@@ -13626,7 +13645,7 @@
       </c>
       <c r="I319" s="20"/>
     </row>
-    <row r="320" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" ht="15">
       <c r="A320" s="20" t="b">
         <v>0</v>
       </c>
@@ -13645,7 +13664,7 @@
       <c r="H320" s="20"/>
       <c r="I320" s="20"/>
     </row>
-    <row r="321" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" ht="15">
       <c r="A321" s="20"/>
       <c r="B321" s="20" t="s">
         <v>24</v>
@@ -13666,7 +13685,7 @@
       <c r="H321" s="20"/>
       <c r="I321" s="20"/>
     </row>
-    <row r="322" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" ht="15">
       <c r="A322" s="20"/>
       <c r="B322" s="20" t="s">
         <v>24</v>
@@ -13687,7 +13706,7 @@
       <c r="H322" s="20"/>
       <c r="I322" s="20"/>
     </row>
-    <row r="323" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" ht="15">
       <c r="A323" s="20"/>
       <c r="B323" s="20" t="s">
         <v>24</v>
@@ -13710,7 +13729,7 @@
       </c>
       <c r="I323" s="20"/>
     </row>
-    <row r="324" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" ht="15">
       <c r="A324" s="20" t="b">
         <v>0</v>
       </c>
@@ -13729,7 +13748,7 @@
       <c r="H324" s="20"/>
       <c r="I324" s="20"/>
     </row>
-    <row r="325" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" ht="15">
       <c r="A325" s="20" t="b">
         <v>0</v>
       </c>
@@ -13748,7 +13767,7 @@
       <c r="H325" s="20"/>
       <c r="I325" s="20"/>
     </row>
-    <row r="326" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" ht="15">
       <c r="A326" s="20"/>
       <c r="B326" s="20" t="s">
         <v>24</v>
@@ -13773,7 +13792,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" ht="15">
       <c r="A327" s="20"/>
       <c r="B327" s="20" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
fix test failure when you don't pass a mean to a discrete variable
</commit_message>
<xml_diff>
--- a/spec/files/discrete_variables.xlsx
+++ b/spec/files/discrete_variables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12820" activeTab="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="491">
   <si>
     <t>type</t>
   </si>
@@ -1497,6 +1497,12 @@
   </si>
   <si>
     <t>(double)</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -1621,7 +1627,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1247">
+  <cellStyleXfs count="1249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2869,8 +2875,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2935,8 +2943,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1247">
+  <cellStyles count="1249">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3560,6 +3569,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1248" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4183,6 +4193,7 @@
     <cellStyle name="Hyperlink" xfId="1241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1247" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4857,9 +4868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5082,10 +5093,18 @@
       <c r="H6">
         <v>30</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>10</v>
+      </c>
+      <c r="L6" s="3">
+        <v>5</v>
+      </c>
+      <c r="M6" s="3">
+        <v>3</v>
+      </c>
       <c r="N6" s="3" t="s">
         <v>474</v>
       </c>
@@ -5577,6 +5596,18 @@
         <v>0</v>
       </c>
       <c r="I23" s="20"/>
+      <c r="J23" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="L23" s="32" t="s">
+        <v>490</v>
+      </c>
+      <c r="M23" s="32" t="s">
+        <v>490</v>
+      </c>
       <c r="N23" t="s">
         <v>481</v>
       </c>
@@ -5911,8 +5942,18 @@
         <v>0</v>
       </c>
       <c r="I36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="3"/>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>90</v>
+      </c>
+      <c r="L36" s="20">
+        <v>30</v>
+      </c>
+      <c r="M36" s="3">
+        <v>3</v>
+      </c>
       <c r="N36" s="3" t="s">
         <v>479</v>
       </c>

</xml_diff>

<commit_message>
move to symbolized header in excel file
</commit_message>
<xml_diff>
--- a/spec/files/discrete_variables.xlsx
+++ b/spec/files/discrete_variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="493">
   <si>
     <t>type</t>
   </si>
@@ -1436,9 +1436,6 @@
     <t>You can change the identifier (which becomes the file name for the zip and json file) and the seed model location.</t>
   </si>
   <si>
-    <t>0.1.10</t>
-  </si>
-  <si>
     <t>Continuous Variable Description</t>
   </si>
   <si>
@@ -1503,6 +1500,15 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>2 Cores</t>
+  </si>
+  <si>
+    <t>$0.410/hour</t>
+  </si>
+  <si>
+    <t>0.1.11</t>
   </si>
 </sst>
 </file>
@@ -4218,57 +4224,12 @@
       <sheetName val="Lookups"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>m2.xlarge</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>2 Cores</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>$0.410/hour</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>m2.2xlarge</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>4 Cores</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>$0.820/hour</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>c3.2xlarge</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>8 Cores</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>$1.20/hour</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>cc2.8xlarge</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>16 Cores</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>$2.40/hour</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4597,8 +4558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4634,7 +4595,7 @@
         <v>452</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>468</v>
+        <v>492</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>453</v>
@@ -4647,13 +4608,11 @@
       <c r="B4" s="25" t="s">
         <v>455</v>
       </c>
-      <c r="C4" s="3" t="str">
-        <f>INDEX([1]Lookups!$A$2:$C$5,MATCH($B4,[1]Lookups!$A$2:$A$5,0),2)</f>
-        <v>2 Cores</v>
-      </c>
-      <c r="D4" s="3" t="str">
-        <f>INDEX([1]Lookups!$A$2:$C$5,MATCH($B4,[1]Lookups!$A$2:$A$5,0),3)</f>
-        <v>$0.410/hour</v>
+      <c r="C4" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>491</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>456</v>
@@ -4666,13 +4625,11 @@
       <c r="B5" s="25" t="s">
         <v>455</v>
       </c>
-      <c r="C5" s="3" t="str">
-        <f>INDEX([1]Lookups!$A$2:$C$5,MATCH($B5,[1]Lookups!$A$2:$A$5,0),2)</f>
-        <v>2 Cores</v>
-      </c>
-      <c r="D5" s="3" t="str">
-        <f>INDEX([1]Lookups!$A$2:$C$5,MATCH($B5,[1]Lookups!$A$2:$A$5,0),3)</f>
-        <v>$0.410/hour</v>
+      <c r="C5" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>491</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>458</v>
@@ -4812,7 +4769,7 @@
         <v>37</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>48</v>
@@ -4868,9 +4825,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomLeft" activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4882,7 +4839,7 @@
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" style="5"/>
     <col min="10" max="13" width="11.5" style="1"/>
     <col min="14" max="14" width="13.6640625" style="1" customWidth="1"/>
@@ -4908,13 +4865,13 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="31" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
       <c r="N1" s="30" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="O1" s="28"/>
       <c r="P1" s="6"/>
@@ -4983,10 +4940,10 @@
         <v>9</v>
       </c>
       <c r="N3" s="18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>8</v>
@@ -5106,16 +5063,16 @@
         <v>3</v>
       </c>
       <c r="N6" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>475</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="R6" s="2"/>
     </row>
@@ -5238,7 +5195,7 @@
       <c r="O10" s="3"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -5597,25 +5554,25 @@
       </c>
       <c r="I23" s="20"/>
       <c r="J23" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="L23" s="32" t="s">
         <v>489</v>
       </c>
-      <c r="K23" s="32" t="s">
+      <c r="M23" s="32" t="s">
         <v>489</v>
       </c>
-      <c r="L23" s="32" t="s">
-        <v>490</v>
-      </c>
-      <c r="M23" s="32" t="s">
-        <v>490</v>
-      </c>
       <c r="N23" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="O23" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="P23" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="24" spans="1:16" customFormat="1" ht="15">
@@ -5948,18 +5905,14 @@
       <c r="K36">
         <v>90</v>
       </c>
-      <c r="L36" s="20">
-        <v>30</v>
-      </c>
-      <c r="M36" s="3">
-        <v>3</v>
-      </c>
+      <c r="L36" s="20"/>
+      <c r="M36" s="3"/>
       <c r="N36" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O36" s="3"/>
       <c r="P36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -6007,19 +5960,19 @@
   <sheetData>
     <row r="1" spans="1:24" ht="18">
       <c r="A1" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>485</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>486</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -6046,10 +5999,10 @@
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>487</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>488</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>

</xml_diff>